<commit_message>
Invincible and Fury Size mode added!
Former-commit-id: 0882a311793ecfd682596a8f7f097c4b9b018b98
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,240 +29,6 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="F50" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Microsoft Office User:Marc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>include scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G50" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Marc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>exclude scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Microsoft Office User:Marc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>include scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G51" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Marc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>exclude scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F52" authorId="0" shapeId="0">
       <text>
         <r>
@@ -326,7 +92,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Marc</t>
         </r>
@@ -336,7 +101,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -348,7 +112,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>exclude scenes</t>
         </r>
@@ -358,7 +121,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -369,19 +131,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
         </r>
         <r>
           <rPr>
@@ -557,6 +308,255 @@
       </text>
     </comment>
     <comment ref="G54" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F55" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G55" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F56" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G56" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="237">
   <si>
     <t>[sku]</t>
   </si>
@@ -1321,6 +1321,30 @@
   </si>
   <si>
     <t>TID_MOD_EASTER_EGG_HUNT_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>invincible</t>
+  </si>
+  <si>
+    <t>fury_size</t>
+  </si>
+  <si>
+    <t>TID_MOD_INVINCIBLE_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_FURY_SIZE_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_INVINCIBLE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TID_MOD_FURY_SIZE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TID_MOD_FURY_SIZE_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_MOD_INVINCIBLE_DESC_SHORT</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1726,6 +1750,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2250,8 +2283,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K54" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K56" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K56"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -2538,10 +2571,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,41 +4187,37 @@
         <v>225</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C50" s="22" t="s">
-        <v>34</v>
+      <c r="B50" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H50" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="I50" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="J50" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="K50" s="24" t="s">
+      <c r="E50" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="J50" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="K50" s="17" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4196,137 +4225,205 @@
       <c r="A51" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>34</v>
+      <c r="B51" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E51" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H51" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="I51" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="J51" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="K51" s="25" t="s">
+      <c r="E51" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="F51" s="36">
+        <v>100</v>
+      </c>
+      <c r="G51" s="36"/>
+      <c r="H51" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="J51" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="K51" s="17" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C52" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C52" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>103</v>
       </c>
       <c r="F52" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G52" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H52" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="I52" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J52" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="K52" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="J53" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="K53" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16" t="s">
+      <c r="G54" s="16"/>
+      <c r="H54" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="I52" s="23" t="s">
+      <c r="I54" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J54" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="K54" s="17" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="31" t="s">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C55" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D55" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E53" s="32" t="s">
+      <c r="E55" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="F53" s="32" t="s">
+      <c r="F55" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G53" s="32" t="s">
+      <c r="G55" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="H53" s="33" t="s">
+      <c r="H55" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="I53" s="33" t="s">
+      <c r="I55" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="J53" s="29" t="s">
+      <c r="J55" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="K53" s="29" t="s">
+      <c r="K55" s="29" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B54" s="31" t="s">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C56" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D56" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E56" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="F54" s="32" t="s">
+      <c r="F56" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="G54" s="32" t="s">
+      <c r="G56" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="H54" s="33" t="s">
+      <c r="H56" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="I54" s="33" t="s">
+      <c r="I56" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="J54" s="29" t="s">
+      <c r="J56" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="K54" s="29" t="s">
+      <c r="K56" s="29" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Chance Improved Mod added in Content for the Pet Shu!
Former-commit-id: ecd8dd4f1a074447710927b75d0cb9804da2ab1e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -29,123 +29,6 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="F52" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Microsoft Office User:Marc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>include scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G52" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Marc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>exclude scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F53" authorId="0" shapeId="0">
       <text>
         <r>
@@ -326,7 +209,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>Marc</t>
         </r>
@@ -336,7 +218,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -348,7 +229,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t>exclude scenes</t>
         </r>
@@ -358,7 +238,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -369,19 +248,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
         </r>
         <r>
           <rPr>
@@ -458,6 +326,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t>Marc</t>
         </r>
@@ -467,6 +336,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -478,6 +348,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t>exclude scenes</t>
         </r>
@@ -487,6 +358,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -497,8 +369,19 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+            <scheme val="minor"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
         </r>
         <r>
           <rPr>
@@ -557,6 +440,123 @@
       </text>
     </comment>
     <comment ref="G56" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F57" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="239">
   <si>
     <t>[sku]</t>
   </si>
@@ -1345,6 +1345,12 @@
   </si>
   <si>
     <t>TID_MOD_INVINCIBLE_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>gatcha_pet_75</t>
+  </si>
+  <si>
+    <t>pet_75</t>
   </si>
 </sst>
 </file>
@@ -2283,8 +2289,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K56" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K57" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K57"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -2571,10 +2577,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,37 +3494,37 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="A29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="8">
-        <v>3</v>
-      </c>
-      <c r="H29" s="8" t="s">
+      <c r="F29" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="G29" s="16">
+        <v>3</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="J29" s="13" t="s">
+      <c r="I29" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="K29" s="13" t="s">
+      <c r="K29" s="17" t="s">
         <v>76</v>
       </c>
     </row>
@@ -3527,7 +3533,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>36</v>
@@ -3539,7 +3545,7 @@
         <v>83</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G30" s="8">
         <v>3</v>
@@ -3548,7 +3554,7 @@
         <v>84</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J30" s="13" t="s">
         <v>86</v>
@@ -3562,7 +3568,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>36</v>
@@ -3574,7 +3580,7 @@
         <v>83</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G31" s="8">
         <v>3</v>
@@ -3583,7 +3589,7 @@
         <v>84</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>86</v>
@@ -3597,7 +3603,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>36</v>
@@ -3609,7 +3615,7 @@
         <v>83</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" s="8">
         <v>3</v>
@@ -3618,7 +3624,7 @@
         <v>84</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>86</v>
@@ -3632,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>36</v>
@@ -3644,7 +3650,7 @@
         <v>83</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="G33" s="8">
         <v>3</v>
@@ -3653,7 +3659,7 @@
         <v>84</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>86</v>
@@ -3667,7 +3673,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>36</v>
@@ -3676,20 +3682,22 @@
         <v>81</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" s="8"/>
+        <v>94</v>
+      </c>
+      <c r="G34" s="8">
+        <v>3</v>
+      </c>
       <c r="H34" s="8" t="s">
-        <v>178</v>
+        <v>84</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>179</v>
+        <v>93</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>180</v>
+        <v>86</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>76</v>
@@ -3700,7 +3708,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>36</v>
@@ -3712,17 +3720,17 @@
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K35" s="13" t="s">
         <v>76</v>
@@ -3733,32 +3741,32 @@
         <v>3</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" s="8">
-        <v>2.1</v>
+        <v>47</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3766,7 +3774,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>33</v>
@@ -3775,20 +3783,20 @@
         <v>82</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F37" s="8">
-        <v>50</v>
+        <v>2.1</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K37" s="13" t="s">
         <v>119</v>
@@ -3799,31 +3807,29 @@
         <v>3</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G38" s="8">
-        <v>80</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F38" s="8">
+        <v>50</v>
+      </c>
+      <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K38" s="13" t="s">
         <v>119</v>
@@ -3834,7 +3840,7 @@
         <v>3</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>34</v>
@@ -3843,22 +3849,22 @@
         <v>82</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
       <c r="G39" s="8">
         <v>80</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K39" s="13" t="s">
         <v>119</v>
@@ -3869,29 +3875,31 @@
         <v>3</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F40" s="8">
-        <v>50</v>
-      </c>
-      <c r="G40" s="8"/>
+        <v>45</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="8">
+        <v>80</v>
+      </c>
       <c r="H40" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K40" s="13" t="s">
         <v>119</v>
@@ -3902,27 +3910,29 @@
         <v>3</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="F41" s="8">
+        <v>50</v>
+      </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K41" s="13" t="s">
         <v>119</v>
@@ -3933,29 +3943,27 @@
         <v>3</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="8">
-        <v>0.46</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K42" s="13" t="s">
         <v>119</v>
@@ -3966,7 +3974,7 @@
         <v>3</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>33</v>
@@ -3975,20 +3983,20 @@
         <v>82</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="F43" s="8">
-        <v>-50</v>
+        <v>0.46</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K43" s="13" t="s">
         <v>119</v>
@@ -3999,7 +4007,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>33</v>
@@ -4011,17 +4019,17 @@
         <v>7</v>
       </c>
       <c r="F44" s="8">
-        <v>30</v>
+        <v>-50</v>
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K44" s="13" t="s">
         <v>119</v>
@@ -4032,7 +4040,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>33</v>
@@ -4041,84 +4049,84 @@
         <v>82</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="F45" s="8">
-        <v>-30</v>
+        <v>30</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="K45" s="13" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C46" s="15" t="s">
+      <c r="A46" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="J46" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="K46" s="17" t="s">
+      <c r="E46" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="8">
+        <v>-30</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="K46" s="13" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" s="27" t="s">
+      <c r="A47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>33</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" s="8">
-        <v>-50</v>
-      </c>
-      <c r="G47" s="8"/>
+      <c r="E47" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
       <c r="H47" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J47" s="17" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K47" s="17" t="s">
         <v>119</v>
@@ -4129,7 +4137,7 @@
         <v>3</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>33</v>
@@ -4138,20 +4146,20 @@
         <v>82</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="F48" s="8">
-        <v>100</v>
+        <v>-50</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="16" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K48" s="17" t="s">
         <v>119</v>
@@ -4162,29 +4170,29 @@
         <v>3</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="F49" s="8">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I49" s="16" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K49" s="17" t="s">
         <v>119</v>
@@ -4194,28 +4202,30 @@
       <c r="A50" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>33</v>
+      <c r="B50" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>34</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
+      <c r="E50" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F50" s="8">
+        <v>75</v>
+      </c>
+      <c r="G50" s="8"/>
       <c r="H50" s="16" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="K50" s="17" t="s">
         <v>119</v>
@@ -4225,30 +4235,28 @@
       <c r="A51" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="C51" s="35" t="s">
+      <c r="B51" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C51" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E51" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="F51" s="36">
-        <v>100</v>
-      </c>
-      <c r="G51" s="36"/>
+        <v>229</v>
+      </c>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
       <c r="H51" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J51" s="17" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K51" s="17" t="s">
         <v>119</v>
@@ -4258,34 +4266,32 @@
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>34</v>
+      <c r="B52" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E52" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H52" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="I52" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="J52" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="K52" s="24" t="s">
+      <c r="E52" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="F52" s="36">
+        <v>100</v>
+      </c>
+      <c r="G52" s="36"/>
+      <c r="H52" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="I52" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="J52" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="K52" s="17" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4294,9 +4300,9 @@
         <v>3</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="7" t="s">
@@ -4306,89 +4312,89 @@
         <v>103</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G53" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="H53" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="I53" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="J53" s="25" t="s">
-        <v>111</v>
-      </c>
-      <c r="K53" s="25" t="s">
+      <c r="H53" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="I53" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J53" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="K53" s="24" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="7" t="s">
         <v>82</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>103</v>
       </c>
       <c r="F54" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="I54" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="J54" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="K54" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F55" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16" t="s">
+      <c r="G55" s="16"/>
+      <c r="H55" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="I54" s="23" t="s">
+      <c r="I55" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="J54" s="17" t="s">
+      <c r="J55" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="K54" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B55" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="C55" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="F55" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="G55" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="H55" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="I55" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="J55" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="K55" s="29" t="s">
+      <c r="K55" s="17" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4397,7 +4403,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C56" s="28" t="s">
         <v>34</v>
@@ -4409,21 +4415,56 @@
         <v>103</v>
       </c>
       <c r="F56" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G56" s="32" t="s">
         <v>136</v>
       </c>
       <c r="H56" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="I56" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="J56" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="K56" s="29" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F57" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G57" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="H57" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="I56" s="33" t="s">
+      <c r="I57" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="J56" s="29" t="s">
+      <c r="J57" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="K56" s="29" t="s">
+      <c r="K57" s="29" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dragon invasion mod fixed.
Former-commit-id: ab3554120f11a7e344139793a0981771b9a1507e
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -634,7 +634,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="238">
   <si>
     <t>[sku]</t>
   </si>
@@ -847,9 +847,6 @@
   </si>
   <si>
     <t>Troll</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>gatcha_pet_33</t>
@@ -2579,8 +2576,8 @@
   </sheetPr>
   <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2618,7 +2615,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>37</v>
@@ -2653,7 +2650,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>38</v>
@@ -2663,16 +2660,16 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="J4" s="13" t="s">
-        <v>147</v>
-      </c>
       <c r="K4" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2686,7 +2683,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>39</v>
@@ -2694,16 +2691,16 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="J5" s="13" t="s">
-        <v>150</v>
-      </c>
       <c r="K5" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2717,7 +2714,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>65</v>
@@ -2727,16 +2724,16 @@
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J6" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>153</v>
-      </c>
       <c r="K6" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2750,7 +2747,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>67</v>
@@ -2760,16 +2757,16 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="J7" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>156</v>
-      </c>
       <c r="K7" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2783,7 +2780,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>42</v>
@@ -2793,16 +2790,16 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>159</v>
-      </c>
       <c r="K8" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2816,7 +2813,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
@@ -2826,16 +2823,16 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>162</v>
-      </c>
       <c r="K9" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2849,7 +2846,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>43</v>
@@ -2859,16 +2856,16 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>165</v>
-      </c>
       <c r="K10" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2882,7 +2879,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>44</v>
@@ -2892,16 +2889,16 @@
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>168</v>
-      </c>
       <c r="K11" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2915,7 +2912,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>66</v>
@@ -2925,16 +2922,16 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="J12" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>171</v>
-      </c>
       <c r="K12" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2948,7 +2945,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>38</v>
@@ -2958,16 +2955,16 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="J13" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>174</v>
-      </c>
       <c r="K13" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2981,7 +2978,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>67</v>
@@ -2991,16 +2988,16 @@
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>177</v>
-      </c>
       <c r="K14" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3008,16 +3005,16 @@
         <v>3</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>11</v>
@@ -3026,16 +3023,16 @@
         <v>3</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="J15" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K15" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3043,16 +3040,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="21" t="s">
         <v>12</v>
@@ -3061,16 +3058,16 @@
         <v>3</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="J16" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K16" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3078,16 +3075,16 @@
         <v>3</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="21" t="s">
         <v>13</v>
@@ -3096,16 +3093,16 @@
         <v>3</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="J17" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K17" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3113,16 +3110,16 @@
         <v>3</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>18</v>
@@ -3131,16 +3128,16 @@
         <v>3</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="J18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J18" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K18" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -3148,16 +3145,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>16</v>
@@ -3166,16 +3163,16 @@
         <v>3</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K19" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3183,16 +3180,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>17</v>
@@ -3201,16 +3198,16 @@
         <v>3</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="J20" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K20" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -3218,16 +3215,16 @@
         <v>3</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>15</v>
@@ -3236,16 +3233,16 @@
         <v>3</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="J21" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J21" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K21" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -3253,16 +3250,16 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>14</v>
@@ -3271,16 +3268,16 @@
         <v>3</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J22" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K22" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -3288,34 +3285,34 @@
         <v>3</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="8">
+        <v>3</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="8">
-        <v>3</v>
-      </c>
-      <c r="H23" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="J23" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J23" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K23" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -3323,34 +3320,34 @@
         <v>3</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" s="8">
+        <v>3</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="8">
-        <v>3</v>
-      </c>
-      <c r="H24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I24" s="8" t="s">
+      <c r="J24" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J24" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K24" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3358,34 +3355,34 @@
         <v>3</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="8">
+        <v>3</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G25" s="8">
-        <v>3</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="8" t="s">
+      <c r="J25" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J25" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K25" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3393,34 +3390,34 @@
         <v>3</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="8">
+        <v>3</v>
+      </c>
+      <c r="H26" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="8">
-        <v>3</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="I26" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="J26" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K26" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3428,34 +3425,34 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="8">
+        <v>3</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="8">
-        <v>3</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="I27" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="J27" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="J27" s="13" t="s">
-        <v>86</v>
-      </c>
       <c r="K27" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3463,34 +3460,34 @@
         <v>3</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="16">
+        <v>3</v>
+      </c>
+      <c r="H28" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" s="16">
-        <v>3</v>
-      </c>
-      <c r="H28" s="16" t="s">
+      <c r="I28" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="J28" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="J28" s="17" t="s">
-        <v>86</v>
-      </c>
       <c r="K28" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -3498,34 +3495,34 @@
         <v>3</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E29" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="G29" s="16">
+        <v>3</v>
+      </c>
+      <c r="H29" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>238</v>
-      </c>
-      <c r="G29" s="16">
-        <v>3</v>
-      </c>
-      <c r="H29" s="16" t="s">
+      <c r="I29" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="J29" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="J29" s="17" t="s">
-        <v>86</v>
-      </c>
       <c r="K29" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3533,34 +3530,34 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E30" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G30" s="8">
+        <v>3</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="G30" s="8">
-        <v>3</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I30" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -3568,34 +3565,34 @@
         <v>3</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31" s="8">
+        <v>3</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G31" s="8">
-        <v>3</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I31" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -3603,34 +3600,34 @@
         <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E32" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" s="8">
+        <v>3</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G32" s="8">
-        <v>3</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I32" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -3638,34 +3635,34 @@
         <v>3</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="8">
+        <v>3</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F33" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G33" s="8">
-        <v>3</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I33" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3673,34 +3670,34 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="8">
+        <v>3</v>
+      </c>
+      <c r="H34" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="G34" s="8">
-        <v>3</v>
-      </c>
-      <c r="H34" s="8" t="s">
-        <v>84</v>
-      </c>
       <c r="I34" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -3714,26 +3711,26 @@
         <v>36</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I35" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="J35" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>180</v>
-      </c>
       <c r="K35" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3747,26 +3744,26 @@
         <v>36</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>47</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="J36" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="J36" s="13" t="s">
-        <v>183</v>
-      </c>
       <c r="K36" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3780,7 +3777,7 @@
         <v>33</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>64</v>
@@ -3790,16 +3787,16 @@
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="I37" s="8" t="s">
+      <c r="J37" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="J37" s="13" t="s">
-        <v>186</v>
-      </c>
       <c r="K37" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3813,7 +3810,7 @@
         <v>33</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>69</v>
@@ -3823,16 +3820,16 @@
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I38" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="I38" s="8" t="s">
+      <c r="J38" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="J38" s="13" t="s">
-        <v>189</v>
-      </c>
       <c r="K38" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -3846,28 +3843,28 @@
         <v>34</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G39" s="8">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H39" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="I39" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="I39" s="8" t="s">
+      <c r="J39" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="J39" s="13" t="s">
-        <v>192</v>
-      </c>
       <c r="K39" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3881,7 +3878,7 @@
         <v>34</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>45</v>
@@ -3890,19 +3887,19 @@
         <v>70</v>
       </c>
       <c r="G40" s="8">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H40" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="J40" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="J40" s="13" t="s">
-        <v>195</v>
-      </c>
       <c r="K40" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3916,7 +3913,7 @@
         <v>33</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>6</v>
@@ -3926,16 +3923,16 @@
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="J41" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="J41" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="K41" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3949,7 +3946,7 @@
         <v>35</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>40</v>
@@ -3957,16 +3954,16 @@
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="I42" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="J42" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="J42" s="13" t="s">
-        <v>201</v>
-      </c>
       <c r="K42" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -3980,7 +3977,7 @@
         <v>33</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>64</v>
@@ -3990,16 +3987,16 @@
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="I43" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="J43" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="J43" s="13" t="s">
-        <v>204</v>
-      </c>
       <c r="K43" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -4013,7 +4010,7 @@
         <v>33</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>7</v>
@@ -4023,16 +4020,16 @@
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="I44" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="J44" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="J44" s="13" t="s">
-        <v>207</v>
-      </c>
       <c r="K44" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -4046,7 +4043,7 @@
         <v>33</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>7</v>
@@ -4056,16 +4053,16 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I45" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="J45" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="J45" s="13" t="s">
-        <v>210</v>
-      </c>
       <c r="K45" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -4079,7 +4076,7 @@
         <v>33</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>69</v>
@@ -4089,16 +4086,16 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I46" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="J46" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="J46" s="13" t="s">
-        <v>213</v>
-      </c>
       <c r="K46" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4112,7 +4109,7 @@
         <v>33</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>41</v>
@@ -4120,16 +4117,16 @@
       <c r="F47" s="16"/>
       <c r="G47" s="16"/>
       <c r="H47" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="I47" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="I47" s="16" t="s">
+      <c r="J47" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="J47" s="17" t="s">
-        <v>216</v>
-      </c>
       <c r="K47" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4143,7 +4140,7 @@
         <v>33</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>65</v>
@@ -4153,16 +4150,16 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="I48" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="I48" s="16" t="s">
+      <c r="J48" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="J48" s="17" t="s">
-        <v>219</v>
-      </c>
       <c r="K48" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -4176,7 +4173,7 @@
         <v>33</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>46</v>
@@ -4186,16 +4183,16 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I49" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="J49" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="J49" s="17" t="s">
-        <v>222</v>
-      </c>
       <c r="K49" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4209,7 +4206,7 @@
         <v>34</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>68</v>
@@ -4219,16 +4216,16 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="I50" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="I50" s="16" t="s">
+      <c r="J50" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="J50" s="17" t="s">
-        <v>225</v>
-      </c>
       <c r="K50" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -4236,30 +4233,30 @@
         <v>3</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C51" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E51" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F51" s="32"/>
       <c r="G51" s="32"/>
       <c r="H51" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I51" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J51" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -4267,32 +4264,32 @@
         <v>3</v>
       </c>
       <c r="B52" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C52" s="35" t="s">
         <v>33</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E52" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F52" s="36">
         <v>100</v>
       </c>
       <c r="G52" s="36"/>
       <c r="H52" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I52" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="J52" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="J52" s="17" t="s">
-        <v>235</v>
-      </c>
       <c r="K52" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -4300,34 +4297,34 @@
         <v>3</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C53" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H53" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="I53" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="I53" s="23" t="s">
+      <c r="J53" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="J53" s="24" t="s">
-        <v>107</v>
-      </c>
       <c r="K53" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -4335,34 +4332,34 @@
         <v>3</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H54" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="I54" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="I54" s="26" t="s">
+      <c r="J54" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="J54" s="25" t="s">
-        <v>111</v>
-      </c>
       <c r="K54" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -4370,32 +4367,32 @@
         <v>3</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I55" s="23" t="s">
         <v>226</v>
       </c>
-      <c r="I55" s="23" t="s">
+      <c r="J55" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="J55" s="17" t="s">
-        <v>228</v>
-      </c>
       <c r="K55" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -4403,34 +4400,34 @@
         <v>3</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F56" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G56" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="H56" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="H56" s="33" t="s">
+      <c r="I56" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="I56" s="33" t="s">
+      <c r="J56" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="J56" s="29" t="s">
-        <v>139</v>
-      </c>
       <c r="K56" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4438,34 +4435,34 @@
         <v>3</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E57" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F57" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G57" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H57" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="I57" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="I57" s="33" t="s">
+      <c r="J57" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="J57" s="29" t="s">
-        <v>142</v>
-      </c>
       <c r="K57" s="29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added present mod and astronaut mode, scenes and content
Former-commit-id: a3330c95f3ac3a0245d5850edb02cc5200f2108b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -629,12 +629,319 @@
         </r>
       </text>
     </comment>
+    <comment ref="G58" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F59" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G59" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="250">
   <si>
     <t>[sku]</t>
   </si>
@@ -1348,6 +1655,42 @@
   </si>
   <si>
     <t>pet_75</t>
+  </si>
+  <si>
+    <t>invasion_TubeMan</t>
+  </si>
+  <si>
+    <t>area2:SP_Medieval_Final_Castle_TubeMan_Invasion</t>
+  </si>
+  <si>
+    <t>TID_MOD_TUBE_MAN_FLOAT_INVASION_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TID_MOD_TUBE_MAN_FLOAT_INVASION_NAME</t>
+  </si>
+  <si>
+    <t>space_goblin_astronaut_invasion</t>
+  </si>
+  <si>
+    <t>TID_MOD_SPACE_GOBLIN_ASTRONAUT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TID_MOD_SPACE_GOBLIN_ASTRONAUT_NAME</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Space_Goblin_Astronaut_Invasion</t>
+  </si>
+  <si>
+    <t>gift_presents_invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Xmas_Gifts_Village,area2:SP_Medieval_Xmas_Gifts_Castle,area3:SP_Medieval_Xmas_Gifts_Dark</t>
+  </si>
+  <si>
+    <t>TID_MOD_GIFT_PRESENT_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_GIFT_PRESENT_DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -2268,8 +2611,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K57" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K60" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K60"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -2556,10 +2899,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K57"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4447,6 +4790,105 @@
         <v>118</v>
       </c>
     </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="G58" s="16"/>
+      <c r="H58" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="I58" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="J58" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="K58" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F59" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="G59" s="16"/>
+      <c r="H59" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="I59" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="J59" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="K59" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F60" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="G60" s="16"/>
+      <c r="H60" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="I60" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="K60" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added space birds mod and alien mod (not loaded)
Former-commit-id: d0e012582e3efff1af42bf21af32e78c5520432c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="mods" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -936,12 +936,392 @@
         </r>
       </text>
     </comment>
+    <comment ref="G61" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G62" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F63" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G63" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F64" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G64" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="259">
   <si>
     <t>[sku]</t>
   </si>
@@ -1261,9 +1641,6 @@
     <t>TID_MOD_GOBLIN_INVASION_1_DESCRIPTION</t>
   </si>
   <si>
-    <t>TID_MOD_GOBLIN_INVASION_1_DESC_SHORT</t>
-  </si>
-  <si>
     <t>goblin_invasion_2</t>
   </si>
   <si>
@@ -1357,18 +1734,12 @@
     <t>TID_MOD_ZOMBIE_INVASION_1_DESCRIPTION</t>
   </si>
   <si>
-    <t>TID_MOD_ZOMBIE_INVASION_1_DESC_SHORT</t>
-  </si>
-  <si>
     <t>TID_MOD_ZOMBIE_INVASION_2_NAME</t>
   </si>
   <si>
     <t>TID_MOD_ZOMBIE_INVASION_2_DESCRIPTION</t>
   </si>
   <si>
-    <t>TID_MOD_ZOMBIE_INVASION_2_DESC_SHORT</t>
-  </si>
-  <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Zombie_Invasion_1,SP_Medieval_Final_Halloween2019;area2:SP_Medieval_Final_Halloween2019</t>
   </si>
   <si>
@@ -1678,9 +2049,6 @@
     <t>TID_MOD_SPACE_GOBLIN_ASTRONAUT_NAME</t>
   </si>
   <si>
-    <t>area1:SP_Medieval_Final_Village_Space_Goblin_Astronaut_Invasion</t>
-  </si>
-  <si>
     <t>gift_presents_invasion</t>
   </si>
   <si>
@@ -1691,6 +2059,45 @@
   </si>
   <si>
     <t>TID_MOD_GIFT_PRESENT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>goblin_Alien_invasion_1</t>
+  </si>
+  <si>
+    <t>goblin_Alien_invasion_2</t>
+  </si>
+  <si>
+    <t>TID_MOD_ALIEN_INVASION_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_ALIEN_INVASION_2_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_ALIEN_INVASION_1_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TID_MOD_ALIEN_INVASION_2_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>space_birds_invasion</t>
+  </si>
+  <si>
+    <t>area2:SP_Medieval_Final_Castle_space_birds_Invasion</t>
+  </si>
+  <si>
+    <t>TID_MOD_SPACE_BIRD_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_SPACE_BIRD_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Space_Goblin_Astronaut_Invasion, area2:SP_Medieval_Final_Castle_Space_Goblin_Astronaut_Invasion</t>
+  </si>
+  <si>
+    <t>space_birds_invasion_spawn</t>
+  </si>
+  <si>
+    <t>space_bird</t>
   </si>
 </sst>
 </file>
@@ -2611,8 +3018,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K60" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K64" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K64"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -2899,10 +3306,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,16 +3392,16 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3016,16 +3423,16 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3049,16 +3456,16 @@
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3082,16 +3489,16 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3115,16 +3522,16 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3148,13 +3555,13 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>76</v>
@@ -3181,13 +3588,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>76</v>
@@ -3214,13 +3621,13 @@
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>76</v>
@@ -3247,13 +3654,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>76</v>
@@ -3280,16 +3687,16 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3313,16 +3720,16 @@
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3715,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>36</v>
@@ -3750,7 +4157,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>36</v>
@@ -3785,7 +4192,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>36</v>
@@ -3820,7 +4227,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>36</v>
@@ -3832,7 +4239,7 @@
         <v>82</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G29" s="16">
         <v>3</v>
@@ -3855,7 +4262,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>36</v>
@@ -3867,7 +4274,7 @@
         <v>82</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G30" s="8">
         <v>3</v>
@@ -3876,7 +4283,7 @@
         <v>83</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J30" s="13" t="s">
         <v>85</v>
@@ -3890,7 +4297,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>36</v>
@@ -3902,7 +4309,7 @@
         <v>82</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G31" s="8">
         <v>3</v>
@@ -3911,7 +4318,7 @@
         <v>83</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>85</v>
@@ -3925,7 +4332,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>36</v>
@@ -3937,7 +4344,7 @@
         <v>82</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G32" s="8">
         <v>3</v>
@@ -3946,7 +4353,7 @@
         <v>83</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J32" s="13" t="s">
         <v>85</v>
@@ -3960,7 +4367,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>36</v>
@@ -3972,7 +4379,7 @@
         <v>82</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G33" s="8">
         <v>3</v>
@@ -3981,7 +4388,7 @@
         <v>83</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J33" s="13" t="s">
         <v>85</v>
@@ -4046,13 +4453,13 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K35" s="13" t="s">
         <v>75</v>
@@ -4079,13 +4486,13 @@
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>75</v>
@@ -4112,16 +4519,16 @@
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4145,16 +4552,16 @@
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K38" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -4174,22 +4581,22 @@
         <v>45</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G39" s="8">
         <v>100</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K39" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -4215,16 +4622,16 @@
         <v>100</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -4248,16 +4655,16 @@
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J41" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K41" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -4279,16 +4686,16 @@
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="J42" s="13" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K42" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -4312,16 +4719,16 @@
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J43" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -4345,16 +4752,16 @@
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -4378,16 +4785,16 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J45" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K45" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -4411,16 +4818,16 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4442,16 +4849,16 @@
       <c r="F47" s="16"/>
       <c r="G47" s="16"/>
       <c r="H47" s="16" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J47" s="17" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4475,16 +4882,16 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I48" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J48" s="17" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -4508,16 +4915,16 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I49" s="16" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J49" s="17" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4541,16 +4948,16 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="16" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J50" s="17" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -4558,7 +4965,7 @@
         <v>3</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>33</v>
@@ -4567,21 +4974,21 @@
         <v>81</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="I51" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="J51" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="J51" s="17" t="s">
-        <v>235</v>
-      </c>
       <c r="K51" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -4589,7 +4996,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>33</v>
@@ -4598,23 +5005,23 @@
         <v>81</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F52" s="32">
         <v>100</v>
       </c>
       <c r="G52" s="32"/>
       <c r="H52" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="I52" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="J52" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="I52" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="J52" s="17" t="s">
-        <v>234</v>
-      </c>
       <c r="K52" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -4634,10 +5041,10 @@
         <v>102</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G53" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H53" s="19" t="s">
         <v>104</v>
@@ -4645,11 +5052,11 @@
       <c r="I53" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="J53" s="20" t="s">
-        <v>106</v>
+      <c r="J53" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="K53" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -4657,7 +5064,7 @@
         <v>3</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>34</v>
@@ -4669,22 +5076,22 @@
         <v>102</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H54" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I54" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="I54" s="22" t="s">
+      <c r="J54" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="J54" s="21" t="s">
-        <v>110</v>
-      </c>
       <c r="K54" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -4692,7 +5099,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>34</v>
@@ -4704,20 +5111,20 @@
         <v>102</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J55" s="17" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -4725,7 +5132,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>34</v>
@@ -4737,22 +5144,22 @@
         <v>102</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G56" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="H56" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="H56" s="29" t="s">
+      <c r="I56" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="I56" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="J56" s="25" t="s">
-        <v>138</v>
+      <c r="J56" s="29" t="s">
+        <v>135</v>
       </c>
       <c r="K56" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -4760,7 +5167,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>34</v>
@@ -4772,22 +5179,22 @@
         <v>102</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G57" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I57" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="J57" s="25" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="J57" s="29" t="s">
+        <v>137</v>
       </c>
       <c r="K57" s="25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -4795,7 +5202,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>34</v>
@@ -4807,20 +5214,20 @@
         <v>102</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="22" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="J58" s="21" t="s">
-        <v>240</v>
+        <v>237</v>
+      </c>
+      <c r="J58" s="22" t="s">
+        <v>238</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4828,7 +5235,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>34</v>
@@ -4840,20 +5247,20 @@
         <v>102</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="22" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4861,7 +5268,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>34</v>
@@ -4873,20 +5280,154 @@
         <v>102</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G60" s="16"/>
       <c r="H60" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="I60" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="K60" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="G61" s="16"/>
+      <c r="H61" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="I61" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="J61" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="K61" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="G62" s="16">
+        <v>100</v>
+      </c>
+      <c r="H62" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="I62" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="J62" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="K62" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C63" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="G63" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H63" s="29" t="s">
         <v>248</v>
       </c>
-      <c r="I60" s="22" t="s">
+      <c r="I63" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="J63" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="K63" s="25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F64" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G64" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="H64" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="J60" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="K60" s="21" t="s">
-        <v>118</v>
+      <c r="I64" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="J64" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="K64" s="25" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added content new mods tournaments quest
Former-commit-id: a51bbca109e7064d76a944b95165268bb185bf04
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -1321,7 +1321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="260">
   <si>
     <t>[sku]</t>
   </si>
@@ -2098,6 +2098,9 @@
   </si>
   <si>
     <t>space_bird</t>
+  </si>
+  <si>
+    <t>Mod iguales a goblin invasion pero al añadir la season de Alien con mascaras, lo unico que cambia en el mod son los TIDS</t>
   </si>
 </sst>
 </file>
@@ -3306,10 +3309,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4894,7 +4897,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>3</v>
       </c>
@@ -4927,7 +4930,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>3</v>
       </c>
@@ -4960,7 +4963,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>3</v>
       </c>
@@ -4991,7 +4994,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
@@ -5024,7 +5027,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
@@ -5059,7 +5062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
@@ -5094,7 +5097,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>3</v>
       </c>
@@ -5127,7 +5130,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>3</v>
       </c>
@@ -5162,7 +5165,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>3</v>
       </c>
@@ -5197,7 +5200,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>3</v>
       </c>
@@ -5230,7 +5233,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>3</v>
       </c>
@@ -5263,7 +5266,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>3</v>
       </c>
@@ -5296,7 +5299,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>3</v>
       </c>
@@ -5329,7 +5332,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
@@ -5364,7 +5367,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="27" t="s">
         <v>246</v>
@@ -5396,8 +5399,11 @@
       <c r="K63" s="25" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="27" t="s">
         <v>247</v>

</xml_diff>

<commit_message>
content mods fixes from merge some disapear
Former-commit-id: 8ae664c7e01f48d1cd54ad49ab52fc8879569a44
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -629,6 +629,50 @@
         </r>
       </text>
     </comment>
+    <comment ref="F58" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G58" authorId="0" shapeId="0">
       <text>
         <r>
@@ -819,7 +863,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F60" authorId="0" shapeId="0">
+    <comment ref="F62" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -860,152 +904,6 @@
             <family val="2"/>
           </rPr>
           <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G60" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Marc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>exclude scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G61" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Marc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>exclude scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
         </r>
       </text>
     </comment>
@@ -1082,7 +980,80 @@
         </r>
       </text>
     </comment>
-    <comment ref="F63" authorId="0" shapeId="0">
+    <comment ref="G63" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1126,7 +1097,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G63" authorId="0" shapeId="0">
+    <comment ref="G72" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1199,7 +1170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F64" authorId="0" shapeId="0">
+    <comment ref="F73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1243,7 +1214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G64" authorId="0" shapeId="0">
+    <comment ref="G73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1321,7 +1292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="279">
   <si>
     <t>[sku]</t>
   </si>
@@ -2088,9 +2059,6 @@
     <t>TID_MOD_SPACE_BIRD_DESCRIPTION</t>
   </si>
   <si>
-    <t>space_birds_invasion_spawn</t>
-  </si>
-  <si>
     <t>space_bird</t>
   </si>
   <si>
@@ -2101,13 +2069,73 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Space_Goblin_Astronaut_Invasion;area2:SP_Medieval_Final_Castle_Space_Goblin_Astronaut_Invasion</t>
+  </si>
+  <si>
+    <t>space_goblin_spawn_100</t>
+  </si>
+  <si>
+    <t>WorkerSpace</t>
+  </si>
+  <si>
+    <t>space_goblin_spawn_95</t>
+  </si>
+  <si>
+    <t>space_birds_spawn_100</t>
+  </si>
+  <si>
+    <t>space_birds_spawn_95</t>
+  </si>
+  <si>
+    <t>invasion_dragon_95</t>
+  </si>
+  <si>
+    <t>invasion_giant_95</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_GHOST_01_PL</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_BURN_ENT_GHOST_03</t>
+  </si>
+  <si>
+    <t>ghost_invasion_100</t>
+  </si>
+  <si>
+    <t>Ghost01;Ghost02;Ghost03</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_BURN_ENT_GHOST_04</t>
+  </si>
+  <si>
+    <t>ghost_invasion_95</t>
+  </si>
+  <si>
+    <t>TID_MOD_INVASION_GHOST_NAME</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_HALLOWEEN_PARCAE_NAME</t>
+  </si>
+  <si>
+    <t>witch_invasion_100</t>
+  </si>
+  <si>
+    <t>BadWitch;GoodWitch;GoodWitch02;Witch</t>
+  </si>
+  <si>
+    <t>TID_MOD_INVASION_WITCH_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_INVASION_WITCH_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>witch_invasion_95</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2198,8 +2226,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2245,6 +2287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2394,7 +2442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2497,6 +2545,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3021,8 +3084,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K64" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K73" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K73"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -3309,10 +3372,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4897,7 +4960,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>3</v>
       </c>
@@ -4930,7 +4993,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>3</v>
       </c>
@@ -4963,7 +5026,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>3</v>
       </c>
@@ -4994,7 +5057,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
@@ -5027,7 +5090,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
@@ -5062,7 +5125,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
@@ -5097,7 +5160,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>3</v>
       </c>
@@ -5130,7 +5193,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>3</v>
       </c>
@@ -5165,7 +5228,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>3</v>
       </c>
@@ -5200,8 +5263,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B58" s="14" t="s">
@@ -5216,7 +5279,7 @@
       <c r="E58" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F58" s="28" t="s">
         <v>236</v>
       </c>
       <c r="G58" s="16"/>
@@ -5233,7 +5296,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>3</v>
       </c>
@@ -5250,7 +5313,7 @@
         <v>102</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="22" t="s">
@@ -5266,12 +5329,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="14" t="s">
-        <v>242</v>
+      <c r="B60" s="37" t="s">
+        <v>259</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>34</v>
@@ -5279,32 +5342,34 @@
       <c r="D60" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E60" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F60" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="G60" s="16"/>
+      <c r="E60" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G60" s="8">
+        <v>100</v>
+      </c>
       <c r="H60" s="22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J60" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="14" t="s">
-        <v>251</v>
+      <c r="B61" s="37" t="s">
+        <v>261</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>34</v>
@@ -5312,32 +5377,34 @@
       <c r="D61" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="G61" s="16"/>
+      <c r="E61" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="G61" s="8">
+        <v>95</v>
+      </c>
       <c r="H61" s="22" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="J61" s="22" t="s">
-        <v>253</v>
+        <v>240</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>241</v>
       </c>
       <c r="K61" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>34</v>
@@ -5345,94 +5412,405 @@
       <c r="D62" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E62" s="8" t="s">
-        <v>45</v>
+      <c r="E62" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="G62" s="16">
-        <v>100</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="G62" s="16"/>
       <c r="H62" s="22" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="J62" s="22" t="s">
-        <v>253</v>
+        <v>244</v>
+      </c>
+      <c r="J62" s="21" t="s">
+        <v>243</v>
       </c>
       <c r="K62" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="27" t="s">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F63" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="G63" s="16"/>
+      <c r="H63" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="I63" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="J63" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="K63" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F64" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="G64" s="8">
+        <v>100</v>
+      </c>
+      <c r="H64" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="I64" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="J64" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="K64" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>263</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="G65" s="8">
+        <v>95</v>
+      </c>
+      <c r="H65" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="I65" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="J65" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="K65" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G66" s="8">
+        <v>95</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J66" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="K66" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G67" s="8">
+        <v>95</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I67" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="K67" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="G68" s="8">
+        <v>100</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="I68" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="J68" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="K68" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="G69" s="8">
+        <v>95</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I69" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="K69" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G70" s="8">
+        <v>100</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I70" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="J70" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="K70" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="G71" s="8">
+        <v>95</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="J71" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="K71" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="B72" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C72" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D63" s="31" t="s">
+      <c r="D72" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E72" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F63" s="28" t="s">
+      <c r="F72" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G63" s="28" t="s">
+      <c r="G72" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="H63" s="29" t="s">
+      <c r="H72" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="I63" s="29" t="s">
+      <c r="I72" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="J63" s="29" t="s">
+      <c r="J72" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="K63" s="25" t="s">
+      <c r="K72" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="M63" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="27" t="s">
+      <c r="M72" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="B73" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C73" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D73" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E64" s="28" t="s">
+      <c r="E73" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="F64" s="28" t="s">
+      <c r="F73" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="G64" s="28" t="s">
+      <c r="G73" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="H64" s="29" t="s">
+      <c r="H73" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="I64" s="29" t="s">
+      <c r="I73" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="J64" s="29" t="s">
+      <c r="J73" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="K64" s="25" t="s">
+      <c r="K73" s="20" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
For rarity eggs mods, added '0' as weight for Baby eggs
Former-commit-id: ec0c3967c0b08bb57aaee04f6ec2dfd069bd55a6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -1525,12 +1525,6 @@
     <t>icon_x2</t>
   </si>
   <si>
-    <t>1;1.4;3</t>
-  </si>
-  <si>
-    <t>1;2;2.2</t>
-  </si>
-  <si>
     <t>[uiCategory]</t>
   </si>
   <si>
@@ -2129,6 +2123,12 @@
   </si>
   <si>
     <t>witch_invasion_95</t>
+  </si>
+  <si>
+    <t>1;2;2.2;0</t>
+  </si>
+  <si>
+    <t>1;1.4;3;0</t>
   </si>
 </sst>
 </file>
@@ -3374,8 +3374,8 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,7 +3413,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>37</v>
@@ -3448,7 +3448,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>38</v>
@@ -3458,16 +3458,16 @@
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>143</v>
-      </c>
       <c r="K4" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -3481,7 +3481,7 @@
         <v>33</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>39</v>
@@ -3489,16 +3489,16 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J5" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>146</v>
-      </c>
       <c r="K5" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -3512,7 +3512,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>65</v>
@@ -3522,16 +3522,16 @@
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>149</v>
-      </c>
       <c r="K6" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -3545,7 +3545,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>67</v>
@@ -3555,16 +3555,16 @@
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>152</v>
-      </c>
       <c r="K7" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -3578,7 +3578,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>42</v>
@@ -3588,16 +3588,16 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>155</v>
-      </c>
       <c r="K8" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -3611,7 +3611,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
@@ -3621,13 +3621,13 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>156</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>76</v>
@@ -3644,7 +3644,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>43</v>
@@ -3654,13 +3654,13 @@
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="J10" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>161</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>76</v>
@@ -3677,7 +3677,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>44</v>
@@ -3687,13 +3687,13 @@
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>162</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>76</v>
@@ -3710,7 +3710,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>66</v>
@@ -3720,13 +3720,13 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="13" t="s">
         <v>165</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>76</v>
@@ -3743,7 +3743,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>38</v>
@@ -3753,16 +3753,16 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>170</v>
-      </c>
       <c r="K13" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3776,7 +3776,7 @@
         <v>33</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>67</v>
@@ -3786,16 +3786,16 @@
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>173</v>
-      </c>
       <c r="K14" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3809,10 +3809,10 @@
         <v>36</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>11</v>
@@ -3821,13 +3821,13 @@
         <v>3</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>75</v>
@@ -3844,10 +3844,10 @@
         <v>36</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F16" s="35" t="s">
         <v>12</v>
@@ -3856,13 +3856,13 @@
         <v>3</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>75</v>
@@ -3879,10 +3879,10 @@
         <v>36</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F17" s="35" t="s">
         <v>13</v>
@@ -3891,13 +3891,13 @@
         <v>3</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>75</v>
@@ -3914,10 +3914,10 @@
         <v>36</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>18</v>
@@ -3926,13 +3926,13 @@
         <v>3</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>75</v>
@@ -3943,16 +3943,16 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>16</v>
@@ -3961,13 +3961,13 @@
         <v>3</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>75</v>
@@ -3978,16 +3978,16 @@
         <v>3</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>17</v>
@@ -3996,13 +3996,13 @@
         <v>3</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>75</v>
@@ -4013,16 +4013,16 @@
         <v>3</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>15</v>
@@ -4031,13 +4031,13 @@
         <v>3</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>75</v>
@@ -4048,16 +4048,16 @@
         <v>3</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>14</v>
@@ -4066,13 +4066,13 @@
         <v>3</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K22" s="13" t="s">
         <v>75</v>
@@ -4083,31 +4083,31 @@
         <v>3</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="F23" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="8">
+        <v>3</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="8">
-        <v>3</v>
-      </c>
-      <c r="H23" s="8" t="s">
+      <c r="J23" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K23" s="13" t="s">
         <v>75</v>
@@ -4118,31 +4118,31 @@
         <v>3</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="F24" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" s="8">
+        <v>3</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="8">
-        <v>3</v>
-      </c>
-      <c r="H24" s="8" t="s">
+      <c r="J24" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>75</v>
@@ -4153,31 +4153,31 @@
         <v>3</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D25" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="8">
+        <v>3</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" s="8">
-        <v>3</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="J25" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>75</v>
@@ -4188,31 +4188,31 @@
         <v>3</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="F26" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="8">
+        <v>3</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="8">
-        <v>3</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="J26" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K26" s="13" t="s">
         <v>75</v>
@@ -4223,31 +4223,31 @@
         <v>3</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="F27" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="8">
+        <v>3</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="8">
-        <v>3</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="J27" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K27" s="13" t="s">
         <v>75</v>
@@ -4258,31 +4258,31 @@
         <v>3</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D28" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="F28" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="16">
+        <v>3</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G28" s="16">
-        <v>3</v>
-      </c>
-      <c r="H28" s="16" t="s">
+      <c r="J28" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>75</v>
@@ -4293,31 +4293,31 @@
         <v>3</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="F29" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="G29" s="16">
+        <v>3</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>234</v>
-      </c>
-      <c r="G29" s="16">
-        <v>3</v>
-      </c>
-      <c r="H29" s="16" t="s">
+      <c r="J29" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>75</v>
@@ -4328,31 +4328,31 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="F30" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G30" s="8">
         <v>3</v>
       </c>
       <c r="H30" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K30" s="13" t="s">
         <v>75</v>
@@ -4363,31 +4363,31 @@
         <v>3</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="F31" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G31" s="8">
         <v>3</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J31" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K31" s="13" t="s">
         <v>75</v>
@@ -4398,31 +4398,31 @@
         <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="F32" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G32" s="8">
         <v>3</v>
       </c>
       <c r="H32" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="J32" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K32" s="13" t="s">
         <v>75</v>
@@ -4433,31 +4433,31 @@
         <v>3</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="F33" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G33" s="8">
         <v>3</v>
       </c>
       <c r="H33" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="J33" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K33" s="13" t="s">
         <v>75</v>
@@ -4468,31 +4468,31 @@
         <v>3</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="F34" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G34" s="8">
         <v>3</v>
       </c>
       <c r="H34" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>85</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>75</v>
@@ -4509,23 +4509,23 @@
         <v>36</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>78</v>
+        <v>277</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="J35" s="13" t="s">
         <v>174</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>176</v>
       </c>
       <c r="K35" s="13" t="s">
         <v>75</v>
@@ -4542,23 +4542,23 @@
         <v>36</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>47</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>77</v>
+        <v>278</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J36" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="K36" s="13" t="s">
         <v>75</v>
@@ -4575,7 +4575,7 @@
         <v>33</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>64</v>
@@ -4585,16 +4585,16 @@
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J37" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="I37" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>182</v>
-      </c>
       <c r="K37" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4608,7 +4608,7 @@
         <v>33</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>69</v>
@@ -4618,16 +4618,16 @@
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J38" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>185</v>
-      </c>
       <c r="K38" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -4641,28 +4641,28 @@
         <v>34</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G39" s="8">
         <v>100</v>
       </c>
       <c r="H39" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J39" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="K39" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -4676,7 +4676,7 @@
         <v>34</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>45</v>
@@ -4688,16 +4688,16 @@
         <v>100</v>
       </c>
       <c r="H40" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="J40" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="I40" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>191</v>
-      </c>
       <c r="K40" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -4711,7 +4711,7 @@
         <v>33</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E41" s="8" t="s">
         <v>6</v>
@@ -4721,16 +4721,16 @@
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="J41" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="I41" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="J41" s="13" t="s">
-        <v>194</v>
-      </c>
       <c r="K41" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -4744,7 +4744,7 @@
         <v>35</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>40</v>
@@ -4752,16 +4752,16 @@
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="J42" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="I42" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>197</v>
-      </c>
       <c r="K42" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -4775,7 +4775,7 @@
         <v>33</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>64</v>
@@ -4785,16 +4785,16 @@
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J43" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="I43" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="J43" s="13" t="s">
-        <v>200</v>
-      </c>
       <c r="K43" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -4808,7 +4808,7 @@
         <v>33</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>7</v>
@@ -4818,16 +4818,16 @@
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="J44" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="I44" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="J44" s="13" t="s">
-        <v>203</v>
-      </c>
       <c r="K44" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -4841,7 +4841,7 @@
         <v>33</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>7</v>
@@ -4851,16 +4851,16 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="I45" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="J45" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="I45" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>206</v>
-      </c>
       <c r="K45" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -4874,7 +4874,7 @@
         <v>33</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>69</v>
@@ -4884,16 +4884,16 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="I46" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J46" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="I46" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="J46" s="13" t="s">
-        <v>209</v>
-      </c>
       <c r="K46" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4907,7 +4907,7 @@
         <v>33</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>41</v>
@@ -4915,16 +4915,16 @@
       <c r="F47" s="16"/>
       <c r="G47" s="16"/>
       <c r="H47" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="J47" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="I47" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="J47" s="17" t="s">
-        <v>212</v>
-      </c>
       <c r="K47" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -4938,7 +4938,7 @@
         <v>33</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>65</v>
@@ -4948,16 +4948,16 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="J48" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="I48" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>215</v>
-      </c>
       <c r="K48" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>33</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>46</v>
@@ -4981,16 +4981,16 @@
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="J49" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="I49" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="J49" s="17" t="s">
-        <v>218</v>
-      </c>
       <c r="K49" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -5004,7 +5004,7 @@
         <v>34</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>68</v>
@@ -5014,16 +5014,16 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="J50" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="I50" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="J50" s="17" t="s">
-        <v>221</v>
-      </c>
       <c r="K50" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -5031,30 +5031,30 @@
         <v>3</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C51" s="24" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="I51" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="I51" s="16" t="s">
-        <v>229</v>
-      </c>
       <c r="J51" s="17" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -5062,32 +5062,32 @@
         <v>3</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>33</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F52" s="32">
         <v>100</v>
       </c>
       <c r="G52" s="32"/>
       <c r="H52" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="I52" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="I52" s="16" t="s">
-        <v>230</v>
-      </c>
       <c r="J52" s="17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K52" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -5095,34 +5095,34 @@
         <v>3</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E53" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G53" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F53" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>104</v>
-      </c>
       <c r="I53" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K53" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -5130,34 +5130,34 @@
         <v>3</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H54" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="J54" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="I54" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>109</v>
-      </c>
       <c r="K54" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -5165,32 +5165,32 @@
         <v>3</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G55" s="16"/>
       <c r="H55" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="I55" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="J55" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="I55" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="J55" s="17" t="s">
-        <v>224</v>
-      </c>
       <c r="K55" s="17" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -5198,34 +5198,34 @@
         <v>3</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C56" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G56" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H56" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="I56" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="H56" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="I56" s="29" t="s">
-        <v>136</v>
-      </c>
       <c r="J56" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K56" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -5233,34 +5233,34 @@
         <v>3</v>
       </c>
       <c r="B57" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C57" s="24" t="s">
         <v>34</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E57" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G57" s="28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H57" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I57" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J57" s="29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K57" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -5268,32 +5268,32 @@
         <v>3</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E58" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -5301,32 +5301,32 @@
         <v>3</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E59" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -5334,34 +5334,34 @@
         <v>3</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G60" s="8">
         <v>100</v>
       </c>
       <c r="H60" s="22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J60" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K60" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -5369,34 +5369,34 @@
         <v>3</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G61" s="8">
         <v>95</v>
       </c>
       <c r="H61" s="22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J61" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="K61" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -5404,32 +5404,32 @@
         <v>3</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E62" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="22" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J62" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -5437,32 +5437,32 @@
         <v>3</v>
       </c>
       <c r="B63" s="38" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J63" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -5470,34 +5470,34 @@
         <v>3</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G64" s="8">
         <v>100</v>
       </c>
       <c r="H64" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J64" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K64" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -5505,34 +5505,34 @@
         <v>3</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G65" s="8">
         <v>95</v>
       </c>
       <c r="H65" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I65" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J65" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="K65" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -5540,34 +5540,34 @@
         <v>3</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G66" s="8">
         <v>95</v>
       </c>
       <c r="H66" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I66" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J66" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="I66" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="J66" s="13" t="s">
-        <v>188</v>
-      </c>
       <c r="K66" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -5575,13 +5575,13 @@
         <v>3</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>45</v>
@@ -5593,16 +5593,16 @@
         <v>95</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J67" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K67" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -5610,34 +5610,34 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G68" s="8">
         <v>100</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J68" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K68" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -5645,34 +5645,34 @@
         <v>3</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G69" s="8">
         <v>95</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K69" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -5680,34 +5680,34 @@
         <v>3</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G70" s="8">
         <v>100</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K70" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -5715,103 +5715,103 @@
         <v>3</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>45</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G71" s="8">
         <v>95</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="K71" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="39" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D72" s="34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E72" s="35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F72" s="40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G72" s="40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H72" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="I72" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="I72" s="19" t="s">
-        <v>249</v>
-      </c>
       <c r="J72" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K72" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M72" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="39" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E73" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F73" s="40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G73" s="40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H73" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="I73" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="I73" s="19" t="s">
-        <v>250</v>
-      </c>
       <c r="J73" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K73" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug mod tid https://mdc-tomcat-jira100.ubisoft.org/jira/browse/HDK-8820
Former-commit-id: 56e9425b408145cbc98202727d5b1ed8f7f29586
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2002,9 +2002,6 @@
     <t>TID_MOD_TUBE_MAN_FLOAT_INVASION_DESCRIPTION</t>
   </si>
   <si>
-    <t>TID_MOD_TUBE_MAN_FLOAT_INVASION_NAME</t>
-  </si>
-  <si>
     <t>space_goblin_astronaut_invasion</t>
   </si>
   <si>
@@ -2129,6 +2126,9 @@
   </si>
   <si>
     <t>1;1.4;3;0</t>
+  </si>
+  <si>
+    <t>TID_MOD_TUBE_MAN_FLOAT_INVASION</t>
   </si>
 </sst>
 </file>
@@ -3374,8 +3374,8 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="G40" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4515,7 +4515,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
@@ -4548,7 +4548,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
@@ -5284,13 +5284,13 @@
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="22" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="I58" s="22" t="s">
         <v>235</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>115</v>
@@ -5301,7 +5301,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>34</v>
@@ -5313,17 +5313,17 @@
         <v>100</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I59" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="J59" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="J59" s="21" t="s">
-        <v>239</v>
       </c>
       <c r="K59" s="21" t="s">
         <v>115</v>
@@ -5334,7 +5334,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>34</v>
@@ -5346,19 +5346,19 @@
         <v>45</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G60" s="8">
         <v>100</v>
       </c>
       <c r="H60" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I60" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="J60" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="J60" s="21" t="s">
-        <v>239</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>115</v>
@@ -5369,7 +5369,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>34</v>
@@ -5381,19 +5381,19 @@
         <v>45</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G61" s="8">
         <v>95</v>
       </c>
       <c r="H61" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I61" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="J61" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="J61" s="21" t="s">
-        <v>239</v>
       </c>
       <c r="K61" s="21" t="s">
         <v>115</v>
@@ -5404,7 +5404,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>34</v>
@@ -5416,17 +5416,17 @@
         <v>100</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="I62" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="I62" s="22" t="s">
-        <v>242</v>
-      </c>
       <c r="J62" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K62" s="21" t="s">
         <v>115</v>
@@ -5437,7 +5437,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>34</v>
@@ -5449,17 +5449,17 @@
         <v>100</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="I63" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="I63" s="22" t="s">
-        <v>252</v>
-      </c>
       <c r="J63" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K63" s="21" t="s">
         <v>115</v>
@@ -5470,7 +5470,7 @@
         <v>3</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>34</v>
@@ -5482,19 +5482,19 @@
         <v>45</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G64" s="8">
         <v>100</v>
       </c>
       <c r="H64" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="I64" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="I64" s="22" t="s">
-        <v>252</v>
-      </c>
       <c r="J64" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K64" s="21" t="s">
         <v>115</v>
@@ -5505,7 +5505,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>34</v>
@@ -5517,19 +5517,19 @@
         <v>45</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G65" s="8">
         <v>95</v>
       </c>
       <c r="H65" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="I65" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="I65" s="22" t="s">
-        <v>252</v>
-      </c>
       <c r="J65" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K65" s="21" t="s">
         <v>115</v>
@@ -5540,7 +5540,7 @@
         <v>3</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>34</v>
@@ -5575,7 +5575,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>34</v>
@@ -5593,13 +5593,13 @@
         <v>95</v>
       </c>
       <c r="H67" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I67" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="I67" s="8" t="s">
-        <v>265</v>
-      </c>
       <c r="J67" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K67" s="13" t="s">
         <v>115</v>
@@ -5610,7 +5610,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>34</v>
@@ -5622,19 +5622,19 @@
         <v>45</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G68" s="8">
         <v>100</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J68" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K68" s="13" t="s">
         <v>115</v>
@@ -5645,7 +5645,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>34</v>
@@ -5657,19 +5657,19 @@
         <v>45</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G69" s="8">
         <v>95</v>
       </c>
       <c r="H69" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="I69" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="I69" s="8" t="s">
-        <v>271</v>
-      </c>
       <c r="J69" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K69" s="13" t="s">
         <v>115</v>
@@ -5680,7 +5680,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>34</v>
@@ -5692,19 +5692,19 @@
         <v>45</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G70" s="8">
         <v>100</v>
       </c>
       <c r="H70" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I70" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="I70" s="8" t="s">
-        <v>275</v>
-      </c>
       <c r="J70" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>115</v>
@@ -5715,7 +5715,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>34</v>
@@ -5727,19 +5727,19 @@
         <v>45</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G71" s="8">
         <v>95</v>
       </c>
       <c r="H71" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="I71" s="8" t="s">
-        <v>275</v>
-      </c>
       <c r="J71" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>115</v>
@@ -5748,7 +5748,7 @@
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>34</v>
@@ -5766,25 +5766,25 @@
         <v>109</v>
       </c>
       <c r="H72" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I72" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J72" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K72" s="20" t="s">
         <v>115</v>
       </c>
       <c r="M72" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>34</v>
@@ -5802,13 +5802,13 @@
         <v>109</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I73" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J73" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K73" s="20" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
fixes TIDS mods ghost 100, giants 95
Former-commit-id: ef5ccdb75e252d778644ce27d92b66270ca44c20
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -1292,7 +1292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="278">
   <si>
     <t>[sku]</t>
   </si>
@@ -2093,9 +2093,6 @@
   </si>
   <si>
     <t>Ghost01;Ghost02;Ghost03</t>
-  </si>
-  <si>
-    <t>TID_QUIP_DRG_BURN_ENT_GHOST_04</t>
   </si>
   <si>
     <t>ghost_invasion_95</t>
@@ -3375,7 +3372,7 @@
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="H67" sqref="H67:J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4515,7 +4512,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
@@ -4548,7 +4545,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
@@ -5284,13 +5281,13 @@
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I58" s="22" t="s">
         <v>235</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>115</v>
@@ -5535,7 +5532,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>3</v>
       </c>
@@ -5593,13 +5590,13 @@
         <v>95</v>
       </c>
       <c r="H67" s="8" t="s">
-        <v>263</v>
+        <v>187</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="J67" s="8" t="s">
-        <v>263</v>
+        <v>188</v>
+      </c>
+      <c r="J67" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="K67" s="13" t="s">
         <v>115</v>
@@ -5631,7 +5628,7 @@
         <v>263</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J68" s="8" t="s">
         <v>263</v>
@@ -5645,7 +5642,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>34</v>
@@ -5663,13 +5660,13 @@
         <v>95</v>
       </c>
       <c r="H69" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I69" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="I69" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="J69" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K69" s="13" t="s">
         <v>115</v>
@@ -5680,7 +5677,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>34</v>
@@ -5692,19 +5689,19 @@
         <v>45</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G70" s="8">
         <v>100</v>
       </c>
       <c r="H70" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I70" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I70" s="8" t="s">
-        <v>274</v>
-      </c>
       <c r="J70" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>115</v>
@@ -5715,7 +5712,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>34</v>
@@ -5727,19 +5724,19 @@
         <v>45</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G71" s="8">
         <v>95</v>
       </c>
       <c r="H71" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="I71" s="8" t="s">
-        <v>274</v>
-      </c>
       <c r="J71" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
fix space birds mod. PF calling name was wrong
Former-commit-id: 8fa48f8003487db6c03c33ca60eaf5f36edd6247
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2050,9 +2050,6 @@
     <t>TID_MOD_SPACE_BIRD_DESCRIPTION</t>
   </si>
   <si>
-    <t>space_bird</t>
-  </si>
-  <si>
     <t>Mod iguales a goblin invasion pero al añadir la season de Alien con mascaras, lo unico que cambia en el mod son los TIDS</t>
   </si>
   <si>
@@ -2126,6 +2123,9 @@
   </si>
   <si>
     <t>TID_MOD_TUBE_MAN_FLOAT_INVASION</t>
+  </si>
+  <si>
+    <t>Canary05_Flock_SPACE</t>
   </si>
 </sst>
 </file>
@@ -3371,8 +3371,8 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67:J67"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4512,7 +4512,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
@@ -4545,7 +4545,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
@@ -5281,13 +5281,13 @@
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I58" s="22" t="s">
         <v>235</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K58" s="21" t="s">
         <v>115</v>
@@ -5310,7 +5310,7 @@
         <v>100</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="22" t="s">
@@ -5331,7 +5331,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>34</v>
@@ -5343,7 +5343,7 @@
         <v>45</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G60" s="8">
         <v>100</v>
@@ -5366,7 +5366,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>34</v>
@@ -5378,7 +5378,7 @@
         <v>45</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G61" s="8">
         <v>95</v>
@@ -5413,7 +5413,7 @@
         <v>100</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="22" t="s">
@@ -5467,7 +5467,7 @@
         <v>3</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>34</v>
@@ -5479,7 +5479,7 @@
         <v>45</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="G64" s="8">
         <v>100</v>
@@ -5502,7 +5502,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>34</v>
@@ -5514,7 +5514,7 @@
         <v>45</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="G65" s="8">
         <v>95</v>
@@ -5537,7 +5537,7 @@
         <v>3</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>34</v>
@@ -5572,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>34</v>
@@ -5607,7 +5607,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>34</v>
@@ -5619,19 +5619,19 @@
         <v>45</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G68" s="8">
         <v>100</v>
       </c>
       <c r="H68" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="I68" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="I68" s="8" t="s">
-        <v>264</v>
-      </c>
       <c r="J68" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K68" s="13" t="s">
         <v>115</v>
@@ -5642,7 +5642,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>34</v>
@@ -5654,19 +5654,19 @@
         <v>45</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G69" s="8">
         <v>95</v>
       </c>
       <c r="H69" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="I69" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="I69" s="8" t="s">
-        <v>269</v>
-      </c>
       <c r="J69" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K69" s="13" t="s">
         <v>115</v>
@@ -5677,7 +5677,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>34</v>
@@ -5689,19 +5689,19 @@
         <v>45</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G70" s="8">
         <v>100</v>
       </c>
       <c r="H70" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="I70" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="I70" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="J70" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>115</v>
@@ -5712,7 +5712,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>34</v>
@@ -5724,19 +5724,19 @@
         <v>45</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G71" s="8">
         <v>95</v>
       </c>
       <c r="H71" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="I71" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="I71" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="J71" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>115</v>
@@ -5777,7 +5777,7 @@
         <v>115</v>
       </c>
       <c r="M72" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed name mod repited qith same name season: Jalapeño to Jalapeno_50
Former-commit-id: e16dfa8cbef10b76b3308cd8267a8c0c26c02960
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2245,9 +2245,6 @@
     <t>TID_MOD_TUBE_MAN_FLOAT_INVASION</t>
   </si>
   <si>
-    <t>jalapeño</t>
-  </si>
-  <si>
     <t>MexicanPepper</t>
   </si>
   <si>
@@ -2255,6 +2252,9 @@
   </si>
   <si>
     <t>LIVE_OPS_50</t>
+  </si>
+  <si>
+    <t>jalapeno_50</t>
   </si>
 </sst>
 </file>
@@ -3500,8 +3500,8 @@
   </sheetPr>
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5949,7 +5949,7 @@
         <v>3</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C74" s="24" t="s">
         <v>34</v>
@@ -5961,19 +5961,19 @@
         <v>45</v>
       </c>
       <c r="F74" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G74" s="28">
         <v>50</v>
       </c>
       <c r="H74" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="I74" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="I74" s="29" t="s">
-        <v>281</v>
-      </c>
       <c r="J74" s="25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K74" s="25" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
adjustments some collisions in CO. Fixed ground point in villager01 because it was floating Pool added cage_zombie, cage_villagers, hangingcage_zombie villager04 moved skull mask new SCENES for mods - Halloween - vampire -werewolves
Former-commit-id: 44ce9d513cf34a12c9c7f115c7dac55af1ee8964
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="mods" sheetId="9" r:id="rId1"/>
@@ -1404,12 +1404,714 @@
         </r>
       </text>
     </comment>
+    <comment ref="F75" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G75" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F77" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G77" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F78" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G78" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F79" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G79" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F80" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G80" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F81" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G81" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="304">
   <si>
     <t>[sku]</t>
   </si>
@@ -2255,6 +2957,72 @@
   </si>
   <si>
     <t>jalapeno_50</t>
+  </si>
+  <si>
+    <t>halloween_invasion_1</t>
+  </si>
+  <si>
+    <t>werewolf_invasion_1</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_1</t>
+  </si>
+  <si>
+    <t>vampire_invasion_1</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Vampire_Invasion_1</t>
+  </si>
+  <si>
+    <t>werewolf_china_invasion_1</t>
+  </si>
+  <si>
+    <t>vampire_china_invasion_1</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Vampire_Invasion_1,SP_Medieval_Final_Halloween2019;area2:SP_Medieval_Final_Halloween2020</t>
+  </si>
+  <si>
+    <t>werewolf_invasion_2</t>
+  </si>
+  <si>
+    <t>werewolf_china_invasion_2</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Halloween_Invasion_1</t>
+  </si>
+  <si>
+    <t>TID_MOD_HALLOWEEN_INVASION_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_HALLOWEEN_INVASION_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_MOD_WEREWOLF_INVASION_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_VAMPIRE_INVASION_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_WEREWOLF_INVASION_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_MOD_WEREWOLF_INVASION_1_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>TID_MOD_VAMPIRE_INVASION_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_MOD_VAMPIRE_INVASION_1_DESC_SHORT</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_2</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_2,SP_Medieval_Final_Halloween2019;area2:SP_Medieval_Final_Halloween2019</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_1,SP_Medieval_Final_Halloween2019;area2:SP_Medieval_Final_Halloween2019</t>
   </si>
 </sst>
 </file>
@@ -3210,8 +3978,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K74" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K81" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K81"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -3498,10 +4266,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3510,7 +4278,7 @@
     <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="57" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
     <col min="6" max="6" width="107" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48.85546875" bestFit="1" customWidth="1"/>
@@ -5979,6 +6747,251 @@
         <v>115</v>
       </c>
     </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F75" s="28" t="s">
+        <v>303</v>
+      </c>
+      <c r="G75" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H75" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="J75" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="K75" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E76" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F76" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="G76" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H76" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="I76" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="J76" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="K76" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F77" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="G77" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H77" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="I77" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="J77" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="K77" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D78" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E78" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F78" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="G78" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H78" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="I78" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="J78" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="K78" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>290</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D79" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E79" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F79" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="G79" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H79" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="I79" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="J79" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="K79" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="C80" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D80" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E80" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F80" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="G80" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H80" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="I80" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="J80" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="K80" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C81" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E81" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F81" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H81" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="I81" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="J81" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="K81" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
night mod content added TBD
Former-commit-id: f11c38cd4c7b3a4be22e8cfbe1953bee3844e3f1
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2223,12 +2223,129 @@
         </r>
       </text>
     </comment>
+    <comment ref="F83" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G83" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="308">
   <si>
     <t>[sku]</t>
   </si>
@@ -3143,6 +3260,15 @@
   </si>
   <si>
     <t>werewolf_only_1</t>
+  </si>
+  <si>
+    <t>night</t>
+  </si>
+  <si>
+    <t>TID_MOD_NIGHT_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_NIGHT_DESC</t>
   </si>
 </sst>
 </file>
@@ -4098,8 +4224,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K82" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K82"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K83" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K83"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -4386,10 +4512,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="G55" workbookViewId="0">
+      <selection activeCell="J83" sqref="J83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7147,6 +7273,37 @@
         <v>115</v>
       </c>
     </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D83" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F83" s="28"/>
+      <c r="G83" s="28"/>
+      <c r="H83" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="I83" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="J83" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="K83" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added werewolf_frank_invasion_1 and 2 using werewolf scene and goblin invasion adjsutmets season mask PF
Former-commit-id: 5520b7ec24a2ed43e3cec53be06d4e26caf40225
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -1989,6 +1989,123 @@
         </r>
       </text>
     </comment>
+    <comment ref="F80" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G80" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F81" authorId="0" shapeId="0">
       <text>
         <r>
@@ -2106,123 +2223,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F82" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Microsoft Office User:Marc
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>include scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G82" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Marc</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>exclude scenes</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F83" authorId="0" shapeId="0">
       <text>
         <r>
@@ -2385,6 +2385,240 @@
       </text>
     </comment>
     <comment ref="G84" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F85" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G85" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F86" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G86" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2462,7 +2696,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="326">
   <si>
     <t>[sku]</t>
   </si>
@@ -3419,13 +3653,34 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Forest;area2:SP_Medieval_Final_Castle_Market</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>werewolf_frank_invasion_1</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_1;area2:SP_Medieval_Final_Castle_Market_Goblin_Invasion_2,ART_Medieval_Final_Castle_Market_Goblin_Invasion_2</t>
+  </si>
+  <si>
+    <t>werewolf_frank_invasion_2</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_1;area2:SP_Medieval_Final_Castle_Market_Goblin_Invasion_1,ART_Medieval_Final_Castle_Market_Goblin_Invasion_1</t>
+  </si>
+  <si>
+    <t>werewolf invasion village forest, goblin frank invasion castle 1</t>
+  </si>
+  <si>
+    <t>werewolf invasion village forest, goblin frank invasion castle 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3528,6 +3783,12 @@
       <color theme="7" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3732,7 +3993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3852,11 +4113,44 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4374,23 +4668,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K84" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:L86" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:L86"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
-  <tableColumns count="11">
-    <tableColumn id="1" name="{modsDefinitions}" dataDxfId="10"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
-    <tableColumn id="3" name="[type]" dataDxfId="8"/>
-    <tableColumn id="11" name="[uiCategory]" dataDxfId="7"/>
-    <tableColumn id="4" name="[target]" dataDxfId="6"/>
-    <tableColumn id="5" name="[param1]" dataDxfId="5"/>
-    <tableColumn id="6" name="[param2]" dataDxfId="4"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="3"/>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="2"/>
-    <tableColumn id="10" name="[tidDescShort]" dataDxfId="1"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="0"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="{modsDefinitions}" dataDxfId="11"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
+    <tableColumn id="3" name="[type]" dataDxfId="9"/>
+    <tableColumn id="11" name="[uiCategory]" dataDxfId="8"/>
+    <tableColumn id="4" name="[target]" dataDxfId="7"/>
+    <tableColumn id="5" name="[param1]" dataDxfId="6"/>
+    <tableColumn id="6" name="[param2]" dataDxfId="5"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="4"/>
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="3"/>
+    <tableColumn id="10" name="[tidDescShort]" dataDxfId="2"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="1"/>
+    <tableColumn id="12" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4662,10 +4957,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4683,7 +4978,7 @@
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -4692,7 +4987,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="93.75" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>49</v>
       </c>
@@ -4726,8 +5021,11 @@
       <c r="K3" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="42" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
@@ -4759,8 +5057,9 @@
       <c r="K4" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="41"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -4790,8 +5089,9 @@
       <c r="K5" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="41"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
@@ -4823,8 +5123,9 @@
       <c r="K6" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="41"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -4856,8 +5157,9 @@
       <c r="K7" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="41"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
@@ -4889,8 +5191,9 @@
       <c r="K8" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="41"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>3</v>
       </c>
@@ -4922,8 +5225,9 @@
       <c r="K9" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="41"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>3</v>
       </c>
@@ -4955,8 +5259,9 @@
       <c r="K10" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="41"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>3</v>
       </c>
@@ -4988,8 +5293,9 @@
       <c r="K11" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="41"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
@@ -5021,8 +5327,9 @@
       <c r="K12" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="41"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>3</v>
       </c>
@@ -5054,8 +5361,9 @@
       <c r="K13" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="41"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>3</v>
       </c>
@@ -5087,8 +5395,9 @@
       <c r="K14" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="41"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>3</v>
       </c>
@@ -5122,8 +5431,9 @@
       <c r="K15" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="41"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>3</v>
       </c>
@@ -5157,8 +5467,9 @@
       <c r="K16" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="41"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>3</v>
       </c>
@@ -5192,8 +5503,9 @@
       <c r="K17" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="41"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>3</v>
       </c>
@@ -5227,8 +5539,9 @@
       <c r="K18" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="41"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>3</v>
       </c>
@@ -5262,8 +5575,9 @@
       <c r="K19" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="41"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>3</v>
       </c>
@@ -5297,8 +5611,9 @@
       <c r="K20" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="41"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>3</v>
       </c>
@@ -5332,8 +5647,9 @@
       <c r="K21" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="41"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>3</v>
       </c>
@@ -5367,8 +5683,9 @@
       <c r="K22" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="41"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>3</v>
       </c>
@@ -5402,8 +5719,9 @@
       <c r="K23" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="41"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>3</v>
       </c>
@@ -5437,8 +5755,9 @@
       <c r="K24" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="41"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
@@ -5472,8 +5791,9 @@
       <c r="K25" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="41"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
@@ -5507,8 +5827,9 @@
       <c r="K26" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="41"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>3</v>
       </c>
@@ -5542,8 +5863,9 @@
       <c r="K27" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="41"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
@@ -5577,8 +5899,9 @@
       <c r="K28" s="17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="41"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -5612,8 +5935,9 @@
       <c r="K29" s="17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="41"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>3</v>
       </c>
@@ -5647,8 +5971,9 @@
       <c r="K30" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="41"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>3</v>
       </c>
@@ -5682,8 +6007,9 @@
       <c r="K31" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="41"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>3</v>
       </c>
@@ -5717,8 +6043,9 @@
       <c r="K32" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="41"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>3</v>
       </c>
@@ -5752,8 +6079,9 @@
       <c r="K33" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="41"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>3</v>
       </c>
@@ -5787,8 +6115,9 @@
       <c r="K34" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="41"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>3</v>
       </c>
@@ -5820,8 +6149,9 @@
       <c r="K35" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="41"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>3</v>
       </c>
@@ -5853,8 +6183,9 @@
       <c r="K36" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="41"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>3</v>
       </c>
@@ -5886,8 +6217,9 @@
       <c r="K37" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="41"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>3</v>
       </c>
@@ -5919,8 +6251,9 @@
       <c r="K38" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="41"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>3</v>
       </c>
@@ -5954,8 +6287,9 @@
       <c r="K39" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="41"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>3</v>
       </c>
@@ -5989,8 +6323,9 @@
       <c r="K40" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="41"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>3</v>
       </c>
@@ -6022,8 +6357,9 @@
       <c r="K41" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="41"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>3</v>
       </c>
@@ -6053,8 +6389,9 @@
       <c r="K42" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="41"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>3</v>
       </c>
@@ -6086,8 +6423,9 @@
       <c r="K43" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="41"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>3</v>
       </c>
@@ -6119,8 +6457,9 @@
       <c r="K44" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="41"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>3</v>
       </c>
@@ -6152,8 +6491,9 @@
       <c r="K45" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="41"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>3</v>
       </c>
@@ -6185,8 +6525,9 @@
       <c r="K46" s="13" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="41"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>3</v>
       </c>
@@ -6216,8 +6557,9 @@
       <c r="K47" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="41"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>3</v>
       </c>
@@ -6249,8 +6591,9 @@
       <c r="K48" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="41"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>3</v>
       </c>
@@ -6282,8 +6625,9 @@
       <c r="K49" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="41"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>3</v>
       </c>
@@ -6315,8 +6659,9 @@
       <c r="K50" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="41"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>3</v>
       </c>
@@ -6346,8 +6691,9 @@
       <c r="K51" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="41"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
@@ -6379,8 +6725,9 @@
       <c r="K52" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="41"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
@@ -6414,8 +6761,9 @@
       <c r="K53" s="20" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53" s="41"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
@@ -6449,8 +6797,9 @@
       <c r="K54" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54" s="41"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>3</v>
       </c>
@@ -6482,8 +6831,9 @@
       <c r="K55" s="17" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55" s="41"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
         <v>3</v>
       </c>
@@ -6517,8 +6867,9 @@
       <c r="K56" s="25" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56" s="41"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
         <v>3</v>
       </c>
@@ -6552,8 +6903,9 @@
       <c r="K57" s="25" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57" s="41"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>3</v>
       </c>
@@ -6585,8 +6937,9 @@
       <c r="K58" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58" s="41"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>3</v>
       </c>
@@ -6618,8 +6971,9 @@
       <c r="K59" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" s="41"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>3</v>
       </c>
@@ -6653,8 +7007,9 @@
       <c r="K60" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60" s="41"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>3</v>
       </c>
@@ -6688,8 +7043,9 @@
       <c r="K61" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61" s="41"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
@@ -6721,8 +7077,9 @@
       <c r="K62" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62" s="41"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>3</v>
       </c>
@@ -6754,8 +7111,9 @@
       <c r="K63" s="21" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63" s="41"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
@@ -6789,6 +7147,7 @@
       <c r="K64" s="21" t="s">
         <v>115</v>
       </c>
+      <c r="L64" s="41"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
@@ -6824,6 +7183,7 @@
       <c r="K65" s="21" t="s">
         <v>115</v>
       </c>
+      <c r="L65" s="41"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
@@ -6859,6 +7219,7 @@
       <c r="K66" s="13" t="s">
         <v>115</v>
       </c>
+      <c r="L66" s="41"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
@@ -6894,6 +7255,7 @@
       <c r="K67" s="13" t="s">
         <v>115</v>
       </c>
+      <c r="L67" s="41"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -6929,6 +7291,7 @@
       <c r="K68" s="13" t="s">
         <v>115</v>
       </c>
+      <c r="L68" s="41"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
@@ -6964,6 +7327,7 @@
       <c r="K69" s="13" t="s">
         <v>115</v>
       </c>
+      <c r="L69" s="41"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
@@ -6999,6 +7363,7 @@
       <c r="K70" s="13" t="s">
         <v>115</v>
       </c>
+      <c r="L70" s="41"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
@@ -7034,6 +7399,7 @@
       <c r="K71" s="13" t="s">
         <v>115</v>
       </c>
+      <c r="L71" s="41"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
@@ -7069,6 +7435,7 @@
       <c r="K72" s="20" t="s">
         <v>115</v>
       </c>
+      <c r="L72" s="41"/>
       <c r="M72" t="s">
         <v>253</v>
       </c>
@@ -7107,6 +7474,7 @@
       <c r="K73" s="20" t="s">
         <v>115</v>
       </c>
+      <c r="L73" s="41"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="26" t="s">
@@ -7142,6 +7510,7 @@
       <c r="K74" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L74" s="41"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="26" t="s">
@@ -7177,11 +7546,14 @@
       <c r="K75" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L75" s="41"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="26"/>
+      <c r="A76" s="26" t="s">
+        <v>3</v>
+      </c>
       <c r="B76" s="27" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>34</v>
@@ -7193,10 +7565,10 @@
         <v>100</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>294</v>
+        <v>323</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>132</v>
+        <v>318</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>288</v>
@@ -7210,13 +7582,17 @@
       <c r="K76" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L76" s="41"/>
+      <c r="M76" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C77" s="24" t="s">
         <v>34</v>
@@ -7228,10 +7604,10 @@
         <v>100</v>
       </c>
       <c r="F77" s="28" t="s">
-        <v>296</v>
+        <v>321</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>132</v>
+        <v>318</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>288</v>
@@ -7244,12 +7620,16 @@
       </c>
       <c r="K77" s="25" t="s">
         <v>115</v>
+      </c>
+      <c r="L77" s="41"/>
+      <c r="M77" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="26"/>
       <c r="B78" s="27" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>34</v>
@@ -7261,7 +7641,7 @@
         <v>100</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G78" s="28" t="s">
         <v>132</v>
@@ -7278,13 +7658,15 @@
       <c r="K78" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L78" s="41"/>
+      <c r="M78" s="43"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>282</v>
+        <v>314</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>34</v>
@@ -7296,30 +7678,29 @@
         <v>100</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="G79" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I79" s="29" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J79" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K79" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L79" s="41"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="26" t="s">
-        <v>3</v>
-      </c>
+      <c r="A80" s="26"/>
       <c r="B80" s="27" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>34</v>
@@ -7331,30 +7712,31 @@
         <v>100</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="G80" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I80" s="29" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J80" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="K80" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L80" s="41"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>34</v>
@@ -7366,30 +7748,31 @@
         <v>100</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>317</v>
+        <v>283</v>
       </c>
       <c r="G81" s="28" t="s">
-        <v>318</v>
+        <v>132</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I81" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="J81" s="25" t="s">
-        <v>286</v>
+        <v>292</v>
+      </c>
+      <c r="J81" s="29" t="s">
+        <v>293</v>
       </c>
       <c r="K81" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L81" s="41"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>34</v>
@@ -7398,33 +7781,34 @@
         <v>79</v>
       </c>
       <c r="E82" s="28" t="s">
-        <v>303</v>
+        <v>100</v>
       </c>
       <c r="F82" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="G82" s="16" t="s">
-        <v>305</v>
+        <v>284</v>
+      </c>
+      <c r="G82" s="28" t="s">
+        <v>132</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="I82" s="29" t="s">
-        <v>302</v>
-      </c>
-      <c r="J82" s="25" t="s">
-        <v>301</v>
+        <v>292</v>
+      </c>
+      <c r="J82" s="29" t="s">
+        <v>293</v>
       </c>
       <c r="K82" s="25" t="s">
         <v>115</v>
       </c>
+      <c r="L82" s="41"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="C83" s="24" t="s">
         <v>34</v>
@@ -7436,31 +7820,31 @@
         <v>100</v>
       </c>
       <c r="F83" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="G83" s="28"/>
+        <v>317</v>
+      </c>
+      <c r="G83" s="28" t="s">
+        <v>318</v>
+      </c>
       <c r="H83" s="29" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="I83" s="29" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="J83" s="25" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
       <c r="K83" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="M83" t="s">
-        <v>309</v>
-      </c>
+      <c r="L83" s="41"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C84" s="24" t="s">
         <v>34</v>
@@ -7469,25 +7853,99 @@
         <v>79</v>
       </c>
       <c r="E84" s="28" t="s">
-        <v>100</v>
+        <v>303</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>313</v>
-      </c>
-      <c r="G84" s="28"/>
+        <v>304</v>
+      </c>
+      <c r="G84" s="16" t="s">
+        <v>305</v>
+      </c>
       <c r="H84" s="29" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="I84" s="29" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="K84" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="M84" t="s">
+      <c r="L84" s="41"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>311</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E85" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F85" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="G85" s="28"/>
+      <c r="H85" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="I85" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="J85" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="K85" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L85" s="41"/>
+      <c r="M85" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="C86" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D86" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="G86" s="28"/>
+      <c r="H86" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="I86" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="J86" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="K86" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L86" s="41"/>
+      <c r="M86" t="s">
         <v>310</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created bat mod: - adding bats - adding bats and replacing some canaries
Former-commit-id: 2b538bb8265a8d16a1444bfd547a7013a2c714ad
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2691,12 +2691,246 @@
         </r>
       </text>
     </comment>
+    <comment ref="F87" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G87" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F88" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G88" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="334">
   <si>
     <t>[sku]</t>
   </si>
@@ -3674,6 +3908,30 @@
   </si>
   <si>
     <t>werewolf invasion village forest, goblin frank invasion castle 2</t>
+  </si>
+  <si>
+    <t>bat_invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Bat_Invasion;area:SP_Medieval_Final_Castle_Bat_Invasion;area3:SP_Medieval_Final_Dark_Bat_Invasion</t>
+  </si>
+  <si>
+    <t>more bats</t>
+  </si>
+  <si>
+    <t>TID_EDIBLE_BAT_PL</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_BATSMALL_03</t>
+  </si>
+  <si>
+    <t>bat_replace_invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Bat_Replace_Invasion,SP_Medieval_Final_Village_Bat_Replace_Invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest,SP_Medieval_Final_Village</t>
   </si>
 </sst>
 </file>
@@ -3993,7 +4251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4121,6 +4379,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4668,8 +4929,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:L86" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:L86"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:L88" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:L88"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -4957,10 +5218,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="N80" sqref="N80"/>
+    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7766,6 +8027,9 @@
         <v>115</v>
       </c>
       <c r="L81" s="41"/>
+      <c r="M81" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="26" t="s">
@@ -7947,6 +8211,82 @@
       <c r="L86" s="41"/>
       <c r="M86" t="s">
         <v>310</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D87" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E87" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F87" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="G87" s="28"/>
+      <c r="H87" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="I87" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="J87" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="K87" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L87" s="44"/>
+      <c r="M87" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="C88" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D88" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E88" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F88" s="28" t="s">
+        <v>332</v>
+      </c>
+      <c r="G88" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="H88" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="I88" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="J88" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="K88" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L88" s="44"/>
+      <c r="M88" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adde scene to content and to Scenes area2:SP_Medieval_Final_Castle_Market_Bat_Invasion
Former-commit-id: c116de1e5a60ff8bd1c0395b711b841fad375434
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -3925,13 +3925,13 @@
     <t>bat_replace_invasion</t>
   </si>
   <si>
-    <t>area1:SP_Medieval_Final_Village_Forest_Bat_Replace_Invasion,SP_Medieval_Final_Village_Bat_Replace_Invasion</t>
-  </si>
-  <si>
     <t>area1:SP_Medieval_Final_Village_Forest,SP_Medieval_Final_Village</t>
   </si>
   <si>
-    <t>area1:SP_Medieval_Final_Village_Forest_Bat_Invasion</t>
+    <t>area1:SP_Medieval_Final_Village_Forest_Bat_Invasion;area2:SP_Medieval_Final_Castle_Market_Bat_Invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Bat_Replace_Invasion,SP_Medieval_Final_Village_Bat_Replace_Invasion;area2:SP_Medieval_Final_Castle_Market_Bat_Invasion</t>
   </si>
 </sst>
 </file>
@@ -5221,7 +5221,7 @@
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8230,7 +8230,7 @@
         <v>100</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="29" t="s">
@@ -8267,10 +8267,10 @@
         <v>100</v>
       </c>
       <c r="F88" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="G88" s="28" t="s">
         <v>331</v>
-      </c>
-      <c r="G88" s="28" t="s">
-        <v>332</v>
       </c>
       <c r="H88" s="29" t="s">
         <v>328</v>

</xml_diff>

<commit_message>
bat 95 mod added
Former-commit-id: 06b3056ed0ba470af45ed4e3635add15949c2b07
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2930,7 +2930,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="338">
   <si>
     <t>[sku]</t>
   </si>
@@ -3932,6 +3932,18 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Bat_Replace_Invasion,SP_Medieval_Final_Village_Bat_Replace_Invasion;area2:SP_Medieval_Final_Castle_Market_Bat_Invasion</t>
+  </si>
+  <si>
+    <t>bats 95%</t>
+  </si>
+  <si>
+    <t>invasion_bat_95</t>
+  </si>
+  <si>
+    <t>BatBig_Flock;BatSmall_Flock</t>
+  </si>
+  <si>
+    <t>TID_QUIP_DRG_KILL_ENT_BATSMALL_02</t>
   </si>
 </sst>
 </file>
@@ -4929,8 +4941,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:L88" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:L88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:L89" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A3:L89"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -5218,10 +5230,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M88"/>
+  <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="F79" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8289,6 +8301,45 @@
         <v>327</v>
       </c>
     </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D89" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E89" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="G89" s="28">
+        <v>95</v>
+      </c>
+      <c r="H89" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="I89" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="J89" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="K89" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L89" s="44"/>
+      <c r="M89" t="s">
+        <v>334</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added more collectable mod
Former-commit-id: 7380a391dad84b5917548a2c9ac732c1c3d7caee
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -2925,12 +2925,100 @@
         </r>
       </text>
     </comment>
+    <comment ref="F90" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F91" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="343">
   <si>
     <t>[sku]</t>
   </si>
@@ -3805,15 +3893,9 @@
     <t>TID_MOD_WEREWOLF_INVASION_1_DESC</t>
   </si>
   <si>
-    <t>TID_MOD_WEREWOLF_INVASION_1_DESC_SHORT</t>
-  </si>
-  <si>
     <t>TID_MOD_VAMPIRE_INVASION_1_DESC</t>
   </si>
   <si>
-    <t>TID_MOD_VAMPIRE_INVASION_1_DESC_SHORT</t>
-  </si>
-  <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Werewolf_Invasion_2</t>
   </si>
   <si>
@@ -3944,6 +4026,27 @@
   </si>
   <si>
     <t>TID_QUIP_DRG_KILL_ENT_BATSMALL_02</t>
+  </si>
+  <si>
+    <t>TID_PET_SEASONAL</t>
+  </si>
+  <si>
+    <t>TID_RESULTS_COLLECTIBLES</t>
+  </si>
+  <si>
+    <t>seasonals_invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Seasonals_Invasion;area2:SP_Medieval_Final_Castle_Market_Seasonals_Invasion;area3:SP_Medieval_Final_Dark_Seasonals_Invasion</t>
+  </si>
+  <si>
+    <t>seasonals_collect_invasion</t>
+  </si>
+  <si>
+    <t>TID_PENDING_REWARDS_COLLECT</t>
+  </si>
+  <si>
+    <t>same but tid diferent</t>
   </si>
 </sst>
 </file>
@@ -4263,7 +4366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4383,47 +4486,27 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <b val="0"/>
@@ -4941,24 +5024,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:L89" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A3:L89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K91" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K91"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
-  <tableColumns count="12">
-    <tableColumn id="1" name="{modsDefinitions}" dataDxfId="11"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="10"/>
-    <tableColumn id="3" name="[type]" dataDxfId="9"/>
-    <tableColumn id="11" name="[uiCategory]" dataDxfId="8"/>
-    <tableColumn id="4" name="[target]" dataDxfId="7"/>
-    <tableColumn id="5" name="[param1]" dataDxfId="6"/>
-    <tableColumn id="6" name="[param2]" dataDxfId="5"/>
-    <tableColumn id="7" name="[tidName]" dataDxfId="4"/>
-    <tableColumn id="8" name="[tidDesc]" dataDxfId="3"/>
-    <tableColumn id="10" name="[tidDescShort]" dataDxfId="2"/>
-    <tableColumn id="9" name="[icon]" dataDxfId="1"/>
-    <tableColumn id="12" name="Column1" dataDxfId="0"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="{modsDefinitions}" dataDxfId="10"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="9"/>
+    <tableColumn id="3" name="[type]" dataDxfId="8"/>
+    <tableColumn id="11" name="[uiCategory]" dataDxfId="7"/>
+    <tableColumn id="4" name="[target]" dataDxfId="6"/>
+    <tableColumn id="5" name="[param1]" dataDxfId="5"/>
+    <tableColumn id="6" name="[param2]" dataDxfId="4"/>
+    <tableColumn id="7" name="[tidName]" dataDxfId="3"/>
+    <tableColumn id="8" name="[tidDesc]" dataDxfId="2"/>
+    <tableColumn id="10" name="[tidDescShort]" dataDxfId="1"/>
+    <tableColumn id="9" name="[icon]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5230,10 +5312,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M89"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F79" workbookViewId="0">
-      <selection activeCell="I89" sqref="I89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5249,6 +5331,7 @@
     <col min="9" max="9" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
@@ -5294,8 +5377,8 @@
       <c r="K3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="42" t="s">
-        <v>319</v>
+      <c r="L3" s="44" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -5330,7 +5413,7 @@
       <c r="K4" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="41"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -5362,7 +5445,7 @@
       <c r="K5" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="45"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -5396,7 +5479,7 @@
       <c r="K6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="41"/>
+      <c r="L6" s="45"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -5430,7 +5513,7 @@
       <c r="K7" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L7" s="41"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -5464,7 +5547,7 @@
       <c r="K8" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L8" s="41"/>
+      <c r="L8" s="45"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -5498,7 +5581,7 @@
       <c r="K9" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="41"/>
+      <c r="L9" s="45"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -5532,7 +5615,7 @@
       <c r="K10" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="41"/>
+      <c r="L10" s="45"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -5566,7 +5649,7 @@
       <c r="K11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L11" s="41"/>
+      <c r="L11" s="45"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -5600,7 +5683,7 @@
       <c r="K12" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="41"/>
+      <c r="L12" s="45"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -5634,7 +5717,7 @@
       <c r="K13" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L13" s="41"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -5668,7 +5751,7 @@
       <c r="K14" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L14" s="41"/>
+      <c r="L14" s="45"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -5704,7 +5787,7 @@
       <c r="K15" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="41"/>
+      <c r="L15" s="45"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -5740,7 +5823,7 @@
       <c r="K16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L16" s="41"/>
+      <c r="L16" s="45"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -5776,7 +5859,7 @@
       <c r="K17" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="41"/>
+      <c r="L17" s="45"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -5812,7 +5895,7 @@
       <c r="K18" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="41"/>
+      <c r="L18" s="45"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
@@ -5848,7 +5931,7 @@
       <c r="K19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L19" s="41"/>
+      <c r="L19" s="45"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -5884,7 +5967,7 @@
       <c r="K20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L20" s="41"/>
+      <c r="L20" s="45"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -5920,7 +6003,7 @@
       <c r="K21" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L21" s="41"/>
+      <c r="L21" s="45"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -5956,7 +6039,7 @@
       <c r="K22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="41"/>
+      <c r="L22" s="45"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -5992,7 +6075,7 @@
       <c r="K23" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L23" s="41"/>
+      <c r="L23" s="45"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
@@ -6028,7 +6111,7 @@
       <c r="K24" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L24" s="41"/>
+      <c r="L24" s="45"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
@@ -6064,7 +6147,7 @@
       <c r="K25" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L25" s="41"/>
+      <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
@@ -6100,7 +6183,7 @@
       <c r="K26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L26" s="41"/>
+      <c r="L26" s="45"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
@@ -6136,7 +6219,7 @@
       <c r="K27" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L27" s="41"/>
+      <c r="L27" s="45"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -6172,7 +6255,7 @@
       <c r="K28" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L28" s="41"/>
+      <c r="L28" s="45"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -6208,7 +6291,7 @@
       <c r="K29" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L29" s="41"/>
+      <c r="L29" s="45"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
@@ -6244,7 +6327,7 @@
       <c r="K30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="41"/>
+      <c r="L30" s="45"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
@@ -6280,7 +6363,7 @@
       <c r="K31" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="41"/>
+      <c r="L31" s="45"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
@@ -6316,7 +6399,7 @@
       <c r="K32" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L32" s="41"/>
+      <c r="L32" s="45"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
@@ -6352,7 +6435,7 @@
       <c r="K33" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L33" s="41"/>
+      <c r="L33" s="45"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
@@ -6388,7 +6471,7 @@
       <c r="K34" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L34" s="41"/>
+      <c r="L34" s="45"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
@@ -6422,7 +6505,7 @@
       <c r="K35" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L35" s="41"/>
+      <c r="L35" s="45"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
@@ -6456,7 +6539,7 @@
       <c r="K36" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L36" s="41"/>
+      <c r="L36" s="45"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
@@ -6490,7 +6573,7 @@
       <c r="K37" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L37" s="41"/>
+      <c r="L37" s="45"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
@@ -6524,7 +6607,7 @@
       <c r="K38" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L38" s="41"/>
+      <c r="L38" s="45"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
@@ -6560,7 +6643,7 @@
       <c r="K39" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L39" s="41"/>
+      <c r="L39" s="45"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -6596,7 +6679,7 @@
       <c r="K40" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L40" s="41"/>
+      <c r="L40" s="45"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
@@ -6630,7 +6713,7 @@
       <c r="K41" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L41" s="41"/>
+      <c r="L41" s="45"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -6662,7 +6745,7 @@
       <c r="K42" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L42" s="41"/>
+      <c r="L42" s="45"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -6696,7 +6779,7 @@
       <c r="K43" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L43" s="41"/>
+      <c r="L43" s="45"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -6730,7 +6813,7 @@
       <c r="K44" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L44" s="41"/>
+      <c r="L44" s="45"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -6764,7 +6847,7 @@
       <c r="K45" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L45" s="41"/>
+      <c r="L45" s="45"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
@@ -6798,7 +6881,7 @@
       <c r="K46" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="41"/>
+      <c r="L46" s="45"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -6830,7 +6913,7 @@
       <c r="K47" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L47" s="41"/>
+      <c r="L47" s="45"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
@@ -6864,7 +6947,7 @@
       <c r="K48" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L48" s="41"/>
+      <c r="L48" s="45"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
@@ -6898,7 +6981,7 @@
       <c r="K49" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L49" s="41"/>
+      <c r="L49" s="45"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
@@ -6932,7 +7015,7 @@
       <c r="K50" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L50" s="41"/>
+      <c r="L50" s="45"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
@@ -6964,7 +7047,7 @@
       <c r="K51" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L51" s="41"/>
+      <c r="L51" s="45"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
@@ -6998,7 +7081,7 @@
       <c r="K52" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L52" s="41"/>
+      <c r="L52" s="45"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
@@ -7034,7 +7117,7 @@
       <c r="K53" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L53" s="41"/>
+      <c r="L53" s="45"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
@@ -7070,7 +7153,7 @@
       <c r="K54" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L54" s="41"/>
+      <c r="L54" s="45"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -7104,7 +7187,7 @@
       <c r="K55" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L55" s="41"/>
+      <c r="L55" s="45"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
@@ -7140,7 +7223,7 @@
       <c r="K56" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L56" s="41"/>
+      <c r="L56" s="45"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
@@ -7176,7 +7259,7 @@
       <c r="K57" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L57" s="41"/>
+      <c r="L57" s="45"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
@@ -7210,7 +7293,7 @@
       <c r="K58" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L58" s="41"/>
+      <c r="L58" s="45"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
@@ -7244,7 +7327,7 @@
       <c r="K59" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L59" s="41"/>
+      <c r="L59" s="45"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
@@ -7280,7 +7363,7 @@
       <c r="K60" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L60" s="41"/>
+      <c r="L60" s="45"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
@@ -7316,7 +7399,7 @@
       <c r="K61" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L61" s="41"/>
+      <c r="L61" s="45"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
@@ -7350,7 +7433,7 @@
       <c r="K62" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L62" s="41"/>
+      <c r="L62" s="45"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
@@ -7384,7 +7467,7 @@
       <c r="K63" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L63" s="41"/>
+      <c r="L63" s="45"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -7420,7 +7503,7 @@
       <c r="K64" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L64" s="41"/>
+      <c r="L64" s="45"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
@@ -7456,7 +7539,7 @@
       <c r="K65" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L65" s="41"/>
+      <c r="L65" s="45"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
@@ -7492,7 +7575,7 @@
       <c r="K66" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L66" s="41"/>
+      <c r="L66" s="45"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
@@ -7528,7 +7611,7 @@
       <c r="K67" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L67" s="41"/>
+      <c r="L67" s="45"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -7556,15 +7639,15 @@
         <v>266</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J68" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K68" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L68" s="41"/>
+      <c r="L68" s="45"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
@@ -7592,15 +7675,15 @@
         <v>266</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K69" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L69" s="41"/>
+      <c r="L69" s="45"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
@@ -7631,12 +7714,12 @@
         <v>270</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L70" s="41"/>
+      <c r="L70" s="45"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
@@ -7667,12 +7750,12 @@
         <v>270</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L71" s="41"/>
+      <c r="L71" s="45"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
@@ -7708,7 +7791,7 @@
       <c r="K72" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L72" s="41"/>
+      <c r="L72" s="45"/>
       <c r="M72" t="s">
         <v>253</v>
       </c>
@@ -7747,7 +7830,7 @@
       <c r="K73" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L73" s="41"/>
+      <c r="L73" s="45"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="26" t="s">
@@ -7783,7 +7866,7 @@
       <c r="K74" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L74" s="41"/>
+      <c r="L74" s="45"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="26" t="s">
@@ -7814,19 +7897,19 @@
         <v>290</v>
       </c>
       <c r="J75" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K75" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L75" s="41"/>
+      <c r="L75" s="45"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B76" s="27" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>34</v>
@@ -7838,10 +7921,10 @@
         <v>100</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G76" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H76" s="29" t="s">
         <v>288</v>
@@ -7850,14 +7933,14 @@
         <v>290</v>
       </c>
       <c r="J76" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K76" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L76" s="41"/>
+      <c r="L76" s="45"/>
       <c r="M76" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -7865,7 +7948,7 @@
         <v>3</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C77" s="24" t="s">
         <v>34</v>
@@ -7877,10 +7960,10 @@
         <v>100</v>
       </c>
       <c r="F77" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G77" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H77" s="29" t="s">
         <v>288</v>
@@ -7889,14 +7972,14 @@
         <v>290</v>
       </c>
       <c r="J77" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K77" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L77" s="41"/>
+      <c r="L77" s="45"/>
       <c r="M77" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -7914,7 +7997,7 @@
         <v>100</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G78" s="28" t="s">
         <v>132</v>
@@ -7926,20 +8009,20 @@
         <v>290</v>
       </c>
       <c r="J78" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K78" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L78" s="41"/>
-      <c r="M78" s="43"/>
+      <c r="L78" s="45"/>
+      <c r="M78" s="41"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>34</v>
@@ -7951,7 +8034,7 @@
         <v>100</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G79" s="28" t="s">
         <v>132</v>
@@ -7963,17 +8046,17 @@
         <v>290</v>
       </c>
       <c r="J79" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K79" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L79" s="41"/>
+      <c r="L79" s="45"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="26"/>
       <c r="B80" s="27" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>34</v>
@@ -7985,7 +8068,7 @@
         <v>100</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G80" s="28" t="s">
         <v>132</v>
@@ -7997,12 +8080,12 @@
         <v>290</v>
       </c>
       <c r="J80" s="29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K80" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L80" s="41"/>
+      <c r="L80" s="45"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="26" t="s">
@@ -8030,17 +8113,17 @@
         <v>289</v>
       </c>
       <c r="I81" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J81" s="29" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="K81" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L81" s="41"/>
+      <c r="L81" s="45"/>
       <c r="M81" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -8048,7 +8131,7 @@
         <v>3</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>34</v>
@@ -8069,15 +8152,15 @@
         <v>289</v>
       </c>
       <c r="I82" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J82" s="29" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="K82" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L82" s="41"/>
+      <c r="L82" s="45"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="26" t="s">
@@ -8096,10 +8179,10 @@
         <v>100</v>
       </c>
       <c r="F83" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G83" s="28" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H83" s="29" t="s">
         <v>286</v>
@@ -8113,14 +8196,14 @@
       <c r="K83" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L83" s="41"/>
+      <c r="L83" s="45"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C84" s="24" t="s">
         <v>34</v>
@@ -8129,34 +8212,34 @@
         <v>79</v>
       </c>
       <c r="E84" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="F84" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="G84" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="F84" s="28" t="s">
-        <v>304</v>
-      </c>
-      <c r="G84" s="16" t="s">
-        <v>305</v>
-      </c>
       <c r="H84" s="29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I84" s="29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K84" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L84" s="41"/>
+      <c r="L84" s="45"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C85" s="24" t="s">
         <v>34</v>
@@ -8168,24 +8251,24 @@
         <v>100</v>
       </c>
       <c r="F85" s="28" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G85" s="28"/>
       <c r="H85" s="29" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I85" s="29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J85" s="25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K85" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L85" s="41"/>
+      <c r="L85" s="45"/>
       <c r="M85" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -8193,7 +8276,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>34</v>
@@ -8205,24 +8288,24 @@
         <v>100</v>
       </c>
       <c r="F86" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G86" s="28"/>
       <c r="H86" s="29" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I86" s="29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="K86" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L86" s="41"/>
+      <c r="L86" s="45"/>
       <c r="M86" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
@@ -8230,7 +8313,7 @@
         <v>3</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C87" s="24" t="s">
         <v>34</v>
@@ -8242,24 +8325,24 @@
         <v>100</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="29" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I87" s="29" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K87" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L87" s="44"/>
+      <c r="L87" s="46"/>
       <c r="M87" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -8267,7 +8350,7 @@
         <v>3</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>34</v>
@@ -8279,26 +8362,26 @@
         <v>100</v>
       </c>
       <c r="F88" s="28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G88" s="28" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H88" s="29" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I88" s="29" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K88" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L88" s="44"/>
+      <c r="L88" s="46"/>
       <c r="M88" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -8306,7 +8389,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C89" s="24" t="s">
         <v>34</v>
@@ -8318,26 +8401,97 @@
         <v>45</v>
       </c>
       <c r="F89" s="28" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G89" s="28">
         <v>95</v>
       </c>
       <c r="H89" s="29" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I89" s="29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="K89" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L89" s="44"/>
+      <c r="L89" s="46"/>
       <c r="M89" t="s">
-        <v>334</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="C90" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D90" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F90" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="G90" s="28"/>
+      <c r="H90" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="I90" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="J90" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="K90" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L90" s="46"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D91" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E91" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F91" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="G91" s="28"/>
+      <c r="H91" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="I91" s="29" t="s">
+        <v>341</v>
+      </c>
+      <c r="J91" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="K91" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L91" s="46"/>
+      <c r="M91" s="42" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change name as it was giving issues in CRM
Former-commit-id: e459eae3a79a47febf7b0d838d4f17a2309dfd12
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -3018,7 +3018,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="344">
   <si>
     <t>[sku]</t>
   </si>
@@ -4047,6 +4047,9 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Seasonals_Invasion;area3:SP_Medieval_Final_Dark_Seasonals_Invasion</t>
+  </si>
+  <si>
+    <t>fury_size_mod</t>
   </si>
 </sst>
 </file>
@@ -5314,8 +5317,8 @@
   </sheetPr>
   <dimension ref="A1:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7054,7 +7057,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>224</v>
+        <v>343</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
added TID night mode
Former-commit-id: 130a86f35782decf206e5c386a2842eabceb3adf
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="8250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="mods" sheetId="9" r:id="rId1"/>
@@ -4151,12 +4151,6 @@
     <t>night</t>
   </si>
   <si>
-    <t>TID_MOD_NIGHT_NAME</t>
-  </si>
-  <si>
-    <t>TID_MOD_NIGHT_DESC</t>
-  </si>
-  <si>
     <t>shader</t>
   </si>
   <si>
@@ -4296,6 +4290,12 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Zombie_Invasion_1</t>
+  </si>
+  <si>
+    <t>TID_POWERUP_DISGUISE_33_NAME</t>
+  </si>
+  <si>
+    <t>TID_QUIP_ENT_DMG_DRG_GHOST_03</t>
   </si>
 </sst>
 </file>
@@ -5563,8 +5563,8 @@
   </sheetPr>
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5627,7 +5627,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -7303,7 +7303,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>33</v>
@@ -7455,7 +7455,7 @@
         <v>100</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G56" s="28" t="s">
         <v>132</v>
@@ -7491,7 +7491,7 @@
         <v>100</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G57" s="28" t="s">
         <v>132</v>
@@ -7515,7 +7515,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>34</v>
@@ -7551,7 +7551,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>34</v>
@@ -8230,7 +8230,7 @@
         <v>3</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>34</v>
@@ -8242,10 +8242,10 @@
         <v>100</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G78" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H78" s="29" t="s">
         <v>288</v>
@@ -8261,7 +8261,7 @@
       </c>
       <c r="L78" s="45"/>
       <c r="M78" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -8269,7 +8269,7 @@
         <v>3</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>34</v>
@@ -8281,10 +8281,10 @@
         <v>100</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G79" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H79" s="29" t="s">
         <v>288</v>
@@ -8300,7 +8300,7 @@
       </c>
       <c r="L79" s="45"/>
       <c r="M79" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -8343,7 +8343,7 @@
         <v>3</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>34</v>
@@ -8377,7 +8377,7 @@
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="26"/>
       <c r="B82" s="27" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>34</v>
@@ -8444,7 +8444,7 @@
       </c>
       <c r="L83" s="45"/>
       <c r="M83" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -8452,7 +8452,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C84" s="24" t="s">
         <v>34</v>
@@ -8500,10 +8500,10 @@
         <v>100</v>
       </c>
       <c r="F85" s="28" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G85" s="28" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H85" s="29" t="s">
         <v>286</v>
@@ -8533,22 +8533,22 @@
         <v>79</v>
       </c>
       <c r="E86" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="G86" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="F86" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="G86" s="16" t="s">
-        <v>303</v>
-      </c>
       <c r="H86" s="29" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
       <c r="I86" s="29" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
       <c r="K86" s="25" t="s">
         <v>115</v>
@@ -8560,7 +8560,7 @@
         <v>3</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C87" s="24" t="s">
         <v>34</v>
@@ -8572,24 +8572,24 @@
         <v>100</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="29" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I87" s="29" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K87" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L87" s="45"/>
       <c r="M87" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -8597,7 +8597,7 @@
         <v>3</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>34</v>
@@ -8609,24 +8609,24 @@
         <v>100</v>
       </c>
       <c r="F88" s="28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G88" s="28"/>
       <c r="H88" s="29" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I88" s="29" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="K88" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L88" s="45"/>
       <c r="M88" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -8634,7 +8634,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C89" s="24" t="s">
         <v>34</v>
@@ -8646,24 +8646,24 @@
         <v>100</v>
       </c>
       <c r="F89" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G89" s="28"/>
       <c r="H89" s="29" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I89" s="29" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K89" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L89" s="46"/>
       <c r="M89" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -8671,7 +8671,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C90" s="24" t="s">
         <v>34</v>
@@ -8683,26 +8683,26 @@
         <v>100</v>
       </c>
       <c r="F90" s="28" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G90" s="28" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="H90" s="29" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I90" s="29" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J90" s="25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K90" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L90" s="46"/>
       <c r="M90" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -8710,7 +8710,7 @@
         <v>3</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C91" s="24" t="s">
         <v>34</v>
@@ -8722,26 +8722,26 @@
         <v>45</v>
       </c>
       <c r="F91" s="28" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G91" s="28">
         <v>95</v>
       </c>
       <c r="H91" s="29" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I91" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K91" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L91" s="46"/>
       <c r="M91" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -8749,7 +8749,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C92" s="24" t="s">
         <v>34</v>
@@ -8761,17 +8761,17 @@
         <v>100</v>
       </c>
       <c r="F92" s="28" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G92" s="28"/>
       <c r="H92" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="I92" s="29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="J92" s="29" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K92" s="25" t="s">
         <v>115</v>
@@ -8783,7 +8783,7 @@
         <v>3</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C93" s="24" t="s">
         <v>34</v>
@@ -8795,24 +8795,24 @@
         <v>100</v>
       </c>
       <c r="F93" s="28" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G93" s="28"/>
       <c r="H93" s="29" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="I93" s="29" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="J93" s="25" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K93" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L93" s="46"/>
       <c r="M93" s="42" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed size villager_01 o normal after halloween mods and tour, quest adjustments added new quest, change mod alien desc tid, added alien quest added halloween hat quest
Former-commit-id: 3ed311593a18dd543b53d845bf99f8dcbb9068dc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -3992,9 +3992,6 @@
     <t>TID_MOD_ALIEN_INVASION_2_NAME</t>
   </si>
   <si>
-    <t>TID_MOD_ALIEN_INVASION_1_DESCRIPTION</t>
-  </si>
-  <si>
     <t>TID_MOD_ALIEN_INVASION_2_DESCRIPTION</t>
   </si>
   <si>
@@ -4296,6 +4293,9 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Zombie_Invasion_1</t>
+  </si>
+  <si>
+    <t>TID_MOD_ALIEN_INVASION_1_DESCRIPTION_2</t>
   </si>
 </sst>
 </file>
@@ -5563,8 +5563,8 @@
   </sheetPr>
   <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5627,7 +5627,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="44" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6739,7 +6739,7 @@
         <v>47</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
@@ -6773,7 +6773,7 @@
         <v>47</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="8" t="s">
@@ -7303,7 +7303,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>33</v>
@@ -7455,7 +7455,7 @@
         <v>100</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G56" s="28" t="s">
         <v>132</v>
@@ -7491,7 +7491,7 @@
         <v>100</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G57" s="28" t="s">
         <v>132</v>
@@ -7515,7 +7515,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>34</v>
@@ -7551,7 +7551,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>34</v>
@@ -7603,13 +7603,13 @@
       </c>
       <c r="G60" s="16"/>
       <c r="H60" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I60" s="22" t="s">
         <v>235</v>
       </c>
       <c r="J60" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K60" s="21" t="s">
         <v>115</v>
@@ -7633,7 +7633,7 @@
         <v>100</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="22" t="s">
@@ -7655,7 +7655,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>34</v>
@@ -7667,7 +7667,7 @@
         <v>45</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G62" s="8">
         <v>100</v>
@@ -7691,7 +7691,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="37" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C63" s="15" t="s">
         <v>34</v>
@@ -7703,7 +7703,7 @@
         <v>45</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G63" s="8">
         <v>95</v>
@@ -7739,7 +7739,7 @@
         <v>100</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="22" t="s">
@@ -7761,7 +7761,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C65" s="15" t="s">
         <v>34</v>
@@ -7773,17 +7773,17 @@
         <v>100</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G65" s="16"/>
       <c r="H65" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="I65" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="I65" s="22" t="s">
-        <v>251</v>
-      </c>
       <c r="J65" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K65" s="21" t="s">
         <v>115</v>
@@ -7795,7 +7795,7 @@
         <v>3</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>34</v>
@@ -7807,19 +7807,19 @@
         <v>45</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G66" s="8">
         <v>100</v>
       </c>
       <c r="H66" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="I66" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="I66" s="22" t="s">
-        <v>251</v>
-      </c>
       <c r="J66" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K66" s="21" t="s">
         <v>115</v>
@@ -7831,7 +7831,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>34</v>
@@ -7843,19 +7843,19 @@
         <v>45</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G67" s="8">
         <v>95</v>
       </c>
       <c r="H67" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="I67" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="I67" s="22" t="s">
-        <v>251</v>
-      </c>
       <c r="J67" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K67" s="21" t="s">
         <v>115</v>
@@ -7867,7 +7867,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>34</v>
@@ -7903,7 +7903,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>34</v>
@@ -7939,7 +7939,7 @@
         <v>3</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>34</v>
@@ -7951,19 +7951,19 @@
         <v>45</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G70" s="8">
         <v>100</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I70" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="J70" s="8" t="s">
         <v>295</v>
-      </c>
-      <c r="J70" s="8" t="s">
-        <v>296</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>115</v>
@@ -7975,7 +7975,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>34</v>
@@ -7987,19 +7987,19 @@
         <v>45</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G71" s="8">
         <v>95</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I71" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="J71" s="8" t="s">
         <v>295</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>296</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>115</v>
@@ -8011,7 +8011,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>34</v>
@@ -8023,19 +8023,19 @@
         <v>45</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G72" s="8">
         <v>100</v>
       </c>
       <c r="H72" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I72" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="I72" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="J72" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K72" s="13" t="s">
         <v>115</v>
@@ -8047,7 +8047,7 @@
         <v>3</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>34</v>
@@ -8059,19 +8059,19 @@
         <v>45</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G73" s="8">
         <v>95</v>
       </c>
       <c r="H73" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="I73" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="I73" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="J73" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K73" s="13" t="s">
         <v>115</v>
@@ -8103,8 +8103,8 @@
       <c r="H74" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="I74" s="19" t="s">
-        <v>246</v>
+      <c r="I74" s="22" t="s">
+        <v>347</v>
       </c>
       <c r="J74" s="19" t="s">
         <v>244</v>
@@ -8114,7 +8114,7 @@
       </c>
       <c r="L74" s="45"/>
       <c r="M74" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -8143,7 +8143,7 @@
         <v>245</v>
       </c>
       <c r="I75" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J75" s="19" t="s">
         <v>245</v>
@@ -8158,7 +8158,7 @@
         <v>3</v>
       </c>
       <c r="B76" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>34</v>
@@ -8170,19 +8170,19 @@
         <v>45</v>
       </c>
       <c r="F76" s="28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G76" s="28">
         <v>50</v>
       </c>
       <c r="H76" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="I76" s="29" t="s">
         <v>276</v>
       </c>
-      <c r="I76" s="29" t="s">
-        <v>277</v>
-      </c>
       <c r="J76" s="25" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K76" s="25" t="s">
         <v>115</v>
@@ -8194,7 +8194,7 @@
         <v>3</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C77" s="24" t="s">
         <v>34</v>
@@ -8206,19 +8206,19 @@
         <v>100</v>
       </c>
       <c r="F77" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G77" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I77" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J77" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K77" s="25" t="s">
         <v>115</v>
@@ -8230,7 +8230,7 @@
         <v>3</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>34</v>
@@ -8242,26 +8242,26 @@
         <v>100</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G78" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H78" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I78" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J78" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K78" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L78" s="45"/>
       <c r="M78" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -8269,7 +8269,7 @@
         <v>3</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>34</v>
@@ -8281,32 +8281,32 @@
         <v>100</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G79" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H79" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I79" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J79" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K79" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L79" s="45"/>
       <c r="M79" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="26"/>
       <c r="B80" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>34</v>
@@ -8318,19 +8318,19 @@
         <v>100</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G80" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H80" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I80" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J80" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K80" s="25" t="s">
         <v>115</v>
@@ -8343,7 +8343,7 @@
         <v>3</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>34</v>
@@ -8355,19 +8355,19 @@
         <v>100</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G81" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I81" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J81" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K81" s="25" t="s">
         <v>115</v>
@@ -8377,7 +8377,7 @@
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="26"/>
       <c r="B82" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>34</v>
@@ -8389,19 +8389,19 @@
         <v>100</v>
       </c>
       <c r="F82" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G82" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I82" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J82" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K82" s="25" t="s">
         <v>115</v>
@@ -8413,7 +8413,7 @@
         <v>3</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C83" s="24" t="s">
         <v>34</v>
@@ -8425,26 +8425,26 @@
         <v>100</v>
       </c>
       <c r="F83" s="28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G83" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I83" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J83" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K83" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L83" s="45"/>
       <c r="M83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -8452,7 +8452,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C84" s="24" t="s">
         <v>34</v>
@@ -8464,19 +8464,19 @@
         <v>100</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G84" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H84" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I84" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J84" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K84" s="25" t="s">
         <v>115</v>
@@ -8488,7 +8488,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C85" s="24" t="s">
         <v>34</v>
@@ -8500,19 +8500,19 @@
         <v>100</v>
       </c>
       <c r="F85" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="G85" s="28" t="s">
         <v>315</v>
       </c>
-      <c r="G85" s="28" t="s">
-        <v>316</v>
-      </c>
       <c r="H85" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="I85" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="I85" s="29" t="s">
-        <v>287</v>
-      </c>
       <c r="J85" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K85" s="25" t="s">
         <v>115</v>
@@ -8524,7 +8524,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>34</v>
@@ -8533,22 +8533,22 @@
         <v>79</v>
       </c>
       <c r="E86" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="F86" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="G86" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="G86" s="16" t="s">
-        <v>303</v>
-      </c>
       <c r="H86" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="I86" s="29" t="s">
         <v>299</v>
       </c>
-      <c r="I86" s="29" t="s">
-        <v>300</v>
-      </c>
       <c r="J86" s="25" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K86" s="25" t="s">
         <v>115</v>
@@ -8560,7 +8560,7 @@
         <v>3</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C87" s="24" t="s">
         <v>34</v>
@@ -8572,24 +8572,24 @@
         <v>100</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="I87" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="I87" s="29" t="s">
-        <v>306</v>
-      </c>
       <c r="J87" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K87" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L87" s="45"/>
       <c r="M87" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -8597,7 +8597,7 @@
         <v>3</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>34</v>
@@ -8609,24 +8609,24 @@
         <v>100</v>
       </c>
       <c r="F88" s="28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G88" s="28"/>
       <c r="H88" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="I88" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="I88" s="29" t="s">
-        <v>306</v>
-      </c>
       <c r="J88" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K88" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L88" s="45"/>
       <c r="M88" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -8634,7 +8634,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C89" s="24" t="s">
         <v>34</v>
@@ -8646,24 +8646,24 @@
         <v>100</v>
       </c>
       <c r="F89" s="28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G89" s="28"/>
       <c r="H89" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="I89" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="I89" s="29" t="s">
-        <v>327</v>
-      </c>
       <c r="J89" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K89" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L89" s="46"/>
       <c r="M89" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -8671,7 +8671,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C90" s="24" t="s">
         <v>34</v>
@@ -8683,26 +8683,26 @@
         <v>100</v>
       </c>
       <c r="F90" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G90" s="28" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H90" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="I90" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="I90" s="29" t="s">
-        <v>327</v>
-      </c>
       <c r="J90" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K90" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L90" s="46"/>
       <c r="M90" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -8710,7 +8710,7 @@
         <v>3</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C91" s="24" t="s">
         <v>34</v>
@@ -8722,26 +8722,26 @@
         <v>45</v>
       </c>
       <c r="F91" s="28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G91" s="28">
         <v>95</v>
       </c>
       <c r="H91" s="29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I91" s="29" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K91" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L91" s="46"/>
       <c r="M91" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -8749,7 +8749,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C92" s="24" t="s">
         <v>34</v>
@@ -8761,17 +8761,17 @@
         <v>100</v>
       </c>
       <c r="F92" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G92" s="28"/>
       <c r="H92" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="I92" s="29" t="s">
         <v>336</v>
       </c>
-      <c r="I92" s="29" t="s">
-        <v>337</v>
-      </c>
       <c r="J92" s="29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K92" s="25" t="s">
         <v>115</v>
@@ -8783,7 +8783,7 @@
         <v>3</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C93" s="24" t="s">
         <v>34</v>
@@ -8795,24 +8795,24 @@
         <v>100</v>
       </c>
       <c r="F93" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G93" s="28"/>
       <c r="H93" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I93" s="29" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J93" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K93" s="25" t="s">
         <v>115</v>
       </c>
       <c r="L93" s="46"/>
       <c r="M93" s="42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added mod villager02_xmas_invasion adjustments xmas mod scene vampire. added elves and present to space
Former-commit-id: 966ed172571db39e03152fde630a2e2556d5cd8b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -3247,12 +3247,129 @@
         </r>
       </text>
     </comment>
+    <comment ref="F94" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G94" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Marc</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>exclude scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">areaX:scene,scene,scene;areaY:scene,scene </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="352">
   <si>
     <t>[sku]</t>
   </si>
@@ -4296,6 +4413,18 @@
   </si>
   <si>
     <t>TID_QUIP_ENT_DMG_DRG_GHOST_03</t>
+  </si>
+  <si>
+    <t>villager02_xmas_invasion</t>
+  </si>
+  <si>
+    <t>TID_MOD_XMAS_INVASION_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_XMAS_INVASION_DESC</t>
+  </si>
+  <si>
+    <t>same scene as vampire but: by a component we disabled: bat and put back bierds, cages, scaffold</t>
   </si>
 </sst>
 </file>
@@ -5273,8 +5402,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K93" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K94" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K94"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -5561,10 +5690,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M94" sqref="M94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8815,6 +8944,45 @@
         <v>339</v>
       </c>
     </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="C94" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E94" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="F94" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="G94" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H94" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="I94" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="J94" s="29" t="s">
+        <v>349</v>
+      </c>
+      <c r="K94" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L94" s="45"/>
+      <c r="M94" t="s">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add mods names in the content: TID_MOD_MORE_COLLECTABLES_DESC TID_MOD_MORE_COLLECTABLES_NAME TID_MOD_BATS_INVASION_NAME TID_MOD_BATS_INVASION_DESC TID_MOD_NIGHT_NAME TID_MOD_NIGHT_DESC
jalapeno_invasion new mod and its Scenes:
area1:SP_Medieval_Final_Village_Forest_Jalapeno_Invasion
area2:SP_Medieval_Final_Castle_Market_Jalapeno_Invasion
area3:SP_Medieval_Final_Dark_Jalapeno_Invasion
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdiez\Documents\client_lfs\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3364,12 +3364,56 @@
         </r>
       </text>
     </comment>
+    <comment ref="F95" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Microsoft Office User:Marc
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>include scenes</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>areaX:scene,scene,scene;areaY:scene,scene</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="358">
   <si>
     <t>[sku]</t>
   </si>
@@ -4199,12 +4243,6 @@
     <t>MexicanPepper</t>
   </si>
   <si>
-    <t>LIVE_OPS_47</t>
-  </si>
-  <si>
-    <t>LIVE_OPS_50</t>
-  </si>
-  <si>
     <t>jalapeno_50</t>
   </si>
   <si>
@@ -4370,12 +4408,6 @@
     <t>BatBig_Flock;BatSmall_Flock</t>
   </si>
   <si>
-    <t>TID_QUIP_DRG_KILL_ENT_BATSMALL_02</t>
-  </si>
-  <si>
-    <t>TID_PET_SEASONAL</t>
-  </si>
-  <si>
     <t>TID_RESULTS_COLLECTIBLES</t>
   </si>
   <si>
@@ -4409,12 +4441,6 @@
     <t>area1:SP_Medieval_Final_Village_Forest_Zombie_Invasion_1</t>
   </si>
   <si>
-    <t>TID_POWERUP_DISGUISE_33_NAME</t>
-  </si>
-  <si>
-    <t>TID_QUIP_ENT_DMG_DRG_GHOST_03</t>
-  </si>
-  <si>
     <t>villager02_xmas_invasion</t>
   </si>
   <si>
@@ -4425,13 +4451,49 @@
   </si>
   <si>
     <t>same scene as vampire but: by a component we disabled: bat and put back bierds, cages, scaffold</t>
+  </si>
+  <si>
+    <t>LIVEOPS_47</t>
+  </si>
+  <si>
+    <t>LIVEOPS_50</t>
+  </si>
+  <si>
+    <t>icon_night</t>
+  </si>
+  <si>
+    <t>added more jalapenos</t>
+  </si>
+  <si>
+    <t>TID_MOD_MORE_COLLECTABLES_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_MORE_COLLECTABLES_DESC</t>
+  </si>
+  <si>
+    <t>TID_MOD_BATS_INVASION_DESC</t>
+  </si>
+  <si>
+    <t>TID_MOD_BATS_INVASION_NAME</t>
+  </si>
+  <si>
+    <t>TID_MOD_NIGHT_DESC</t>
+  </si>
+  <si>
+    <t>TID_MOD_NIGHT_NAME</t>
+  </si>
+  <si>
+    <t>jalapeno_invasion</t>
+  </si>
+  <si>
+    <t>area1:SP_Medieval_Final_Village_Forest_Jalapeno_Invasion;area2:SP_Medieval_Final_Castle_Market_Jalapeno_Invasion;area3:SP_Medieval_Final_Dark_Jalapeno_Invasion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4523,23 +4585,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="14"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="7" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4852,12 +4906,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4871,13 +4919,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5402,8 +5456,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K94" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K95" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K95"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -5690,10 +5744,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M94" sqref="M94"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95:J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5709,7 +5763,7 @@
     <col min="9" max="9" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="43"/>
+    <col min="12" max="12" width="8.85546875" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
@@ -5755,8 +5809,8 @@
       <c r="K3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="44" t="s">
-        <v>315</v>
+      <c r="L3" s="42" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -5791,7 +5845,7 @@
       <c r="K4" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -5823,7 +5877,7 @@
       <c r="K5" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L5" s="45"/>
+      <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -5857,7 +5911,7 @@
       <c r="K6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="45"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -5891,7 +5945,7 @@
       <c r="K7" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L7" s="45"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -5925,7 +5979,7 @@
       <c r="K8" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L8" s="45"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -5959,7 +6013,7 @@
       <c r="K9" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="45"/>
+      <c r="L9" s="43"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -5993,7 +6047,7 @@
       <c r="K10" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="43"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
@@ -6027,7 +6081,7 @@
       <c r="K11" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L11" s="45"/>
+      <c r="L11" s="43"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -6061,7 +6115,7 @@
       <c r="K12" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="45"/>
+      <c r="L12" s="43"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -6095,7 +6149,7 @@
       <c r="K13" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L13" s="45"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -6129,7 +6183,7 @@
       <c r="K14" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L14" s="45"/>
+      <c r="L14" s="43"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
@@ -6165,7 +6219,7 @@
       <c r="K15" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="45"/>
+      <c r="L15" s="43"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -6201,7 +6255,7 @@
       <c r="K16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="43"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -6237,7 +6291,7 @@
       <c r="K17" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L17" s="45"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
@@ -6273,7 +6327,7 @@
       <c r="K18" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="45"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
@@ -6309,7 +6363,7 @@
       <c r="K19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L19" s="45"/>
+      <c r="L19" s="43"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -6345,7 +6399,7 @@
       <c r="K20" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L20" s="45"/>
+      <c r="L20" s="43"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -6381,7 +6435,7 @@
       <c r="K21" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L21" s="45"/>
+      <c r="L21" s="43"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -6417,7 +6471,7 @@
       <c r="K22" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="43"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -6453,7 +6507,7 @@
       <c r="K23" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L23" s="45"/>
+      <c r="L23" s="43"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
@@ -6489,7 +6543,7 @@
       <c r="K24" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L24" s="45"/>
+      <c r="L24" s="43"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
@@ -6525,7 +6579,7 @@
       <c r="K25" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L25" s="45"/>
+      <c r="L25" s="43"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
@@ -6561,7 +6615,7 @@
       <c r="K26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L26" s="45"/>
+      <c r="L26" s="43"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
@@ -6597,7 +6651,7 @@
       <c r="K27" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L27" s="45"/>
+      <c r="L27" s="43"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -6633,7 +6687,7 @@
       <c r="K28" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L28" s="45"/>
+      <c r="L28" s="43"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -6669,7 +6723,7 @@
       <c r="K29" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="L29" s="45"/>
+      <c r="L29" s="43"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
@@ -6705,7 +6759,7 @@
       <c r="K30" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L30" s="45"/>
+      <c r="L30" s="43"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
@@ -6741,7 +6795,7 @@
       <c r="K31" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L31" s="45"/>
+      <c r="L31" s="43"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
@@ -6777,7 +6831,7 @@
       <c r="K32" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L32" s="45"/>
+      <c r="L32" s="43"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
@@ -6813,7 +6867,7 @@
       <c r="K33" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L33" s="45"/>
+      <c r="L33" s="43"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
@@ -6849,7 +6903,7 @@
       <c r="K34" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L34" s="45"/>
+      <c r="L34" s="43"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
@@ -6883,7 +6937,7 @@
       <c r="K35" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L35" s="45"/>
+      <c r="L35" s="43"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
@@ -6917,7 +6971,7 @@
       <c r="K36" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="L36" s="45"/>
+      <c r="L36" s="43"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
@@ -6951,7 +7005,7 @@
       <c r="K37" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L37" s="45"/>
+      <c r="L37" s="43"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
@@ -6985,7 +7039,7 @@
       <c r="K38" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L38" s="45"/>
+      <c r="L38" s="43"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
@@ -7021,7 +7075,7 @@
       <c r="K39" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L39" s="45"/>
+      <c r="L39" s="43"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -7057,7 +7111,7 @@
       <c r="K40" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L40" s="45"/>
+      <c r="L40" s="43"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
@@ -7091,7 +7145,7 @@
       <c r="K41" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L41" s="45"/>
+      <c r="L41" s="43"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -7123,7 +7177,7 @@
       <c r="K42" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L42" s="45"/>
+      <c r="L42" s="43"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -7157,7 +7211,7 @@
       <c r="K43" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L43" s="45"/>
+      <c r="L43" s="43"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -7191,7 +7245,7 @@
       <c r="K44" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L44" s="45"/>
+      <c r="L44" s="43"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -7225,7 +7279,7 @@
       <c r="K45" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L45" s="45"/>
+      <c r="L45" s="43"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
@@ -7259,7 +7313,7 @@
       <c r="K46" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L46" s="45"/>
+      <c r="L46" s="43"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -7291,7 +7345,7 @@
       <c r="K47" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L47" s="45"/>
+      <c r="L47" s="43"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
@@ -7325,7 +7379,7 @@
       <c r="K48" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L48" s="45"/>
+      <c r="L48" s="43"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
@@ -7359,7 +7413,7 @@
       <c r="K49" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L49" s="45"/>
+      <c r="L49" s="43"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
@@ -7393,7 +7447,7 @@
       <c r="K50" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L50" s="45"/>
+      <c r="L50" s="43"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
@@ -7425,14 +7479,14 @@
       <c r="K51" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L51" s="45"/>
+      <c r="L51" s="43"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C52" s="31" t="s">
         <v>33</v>
@@ -7459,7 +7513,7 @@
       <c r="K52" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L52" s="45"/>
+      <c r="L52" s="43"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
@@ -7495,7 +7549,7 @@
       <c r="K53" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L53" s="45"/>
+      <c r="L53" s="43"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
@@ -7531,7 +7585,7 @@
       <c r="K54" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L54" s="45"/>
+      <c r="L54" s="43"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -7565,7 +7619,7 @@
       <c r="K55" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="L55" s="45"/>
+      <c r="L55" s="43"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="26" t="s">
@@ -7584,7 +7638,7 @@
         <v>100</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G56" s="28" t="s">
         <v>132</v>
@@ -7601,7 +7655,7 @@
       <c r="K56" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L56" s="45"/>
+      <c r="L56" s="43"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="26" t="s">
@@ -7620,7 +7674,7 @@
         <v>100</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="G57" s="28" t="s">
         <v>132</v>
@@ -7637,14 +7691,14 @@
       <c r="K57" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L57" s="45"/>
+      <c r="L57" s="43"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>34</v>
@@ -7673,14 +7727,14 @@
       <c r="K58" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L58" s="45"/>
+      <c r="L58" s="43"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>34</v>
@@ -7709,7 +7763,7 @@
       <c r="K59" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L59" s="45"/>
+      <c r="L59" s="43"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
@@ -7743,13 +7797,13 @@
       <c r="K60" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L60" s="45"/>
+      <c r="L60" s="43"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="45" t="s">
         <v>236</v>
       </c>
       <c r="C61" s="15" t="s">
@@ -7777,13 +7831,13 @@
       <c r="K61" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L61" s="45"/>
+      <c r="L61" s="43"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="45" t="s">
         <v>256</v>
       </c>
       <c r="C62" s="15" t="s">
@@ -7813,13 +7867,13 @@
       <c r="K62" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L62" s="45"/>
+      <c r="L62" s="43"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="37" t="s">
+      <c r="B63" s="45" t="s">
         <v>258</v>
       </c>
       <c r="C63" s="15" t="s">
@@ -7849,13 +7903,13 @@
       <c r="K63" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L63" s="45"/>
+      <c r="L63" s="43"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="45" t="s">
         <v>239</v>
       </c>
       <c r="C64" s="15" t="s">
@@ -7883,13 +7937,13 @@
       <c r="K64" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L64" s="45"/>
+      <c r="L64" s="43"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="45" t="s">
         <v>248</v>
       </c>
       <c r="C65" s="15" t="s">
@@ -7917,13 +7971,13 @@
       <c r="K65" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L65" s="45"/>
+      <c r="L65" s="43"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="45" t="s">
         <v>259</v>
       </c>
       <c r="C66" s="15" t="s">
@@ -7953,13 +8007,13 @@
       <c r="K66" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L66" s="45"/>
+      <c r="L66" s="43"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B67" s="45" t="s">
         <v>260</v>
       </c>
       <c r="C67" s="15" t="s">
@@ -7989,7 +8043,7 @@
       <c r="K67" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="L67" s="45"/>
+      <c r="L67" s="43"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -8025,7 +8079,7 @@
       <c r="K68" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L68" s="45"/>
+      <c r="L68" s="43"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
@@ -8061,7 +8115,7 @@
       <c r="K69" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L69" s="45"/>
+      <c r="L69" s="43"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
@@ -8089,15 +8143,15 @@
         <v>266</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J70" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K70" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L70" s="45"/>
+      <c r="L70" s="43"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
@@ -8125,15 +8179,15 @@
         <v>266</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J71" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K71" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L71" s="45"/>
+      <c r="L71" s="43"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
@@ -8164,12 +8218,12 @@
         <v>270</v>
       </c>
       <c r="J72" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K72" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L72" s="45"/>
+      <c r="L72" s="43"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
@@ -8200,18 +8254,18 @@
         <v>270</v>
       </c>
       <c r="J73" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K73" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="L73" s="45"/>
+      <c r="L73" s="43"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B74" s="39" t="s">
+      <c r="B74" s="37" t="s">
         <v>242</v>
       </c>
       <c r="C74" s="18" t="s">
@@ -8226,7 +8280,7 @@
       <c r="F74" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="G74" s="40" t="s">
+      <c r="G74" s="38" t="s">
         <v>109</v>
       </c>
       <c r="H74" s="19" t="s">
@@ -8241,7 +8295,7 @@
       <c r="K74" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L74" s="45"/>
+      <c r="L74" s="43"/>
       <c r="M74" t="s">
         <v>253</v>
       </c>
@@ -8250,7 +8304,7 @@
       <c r="A75" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="39" t="s">
+      <c r="B75" s="37" t="s">
         <v>243</v>
       </c>
       <c r="C75" s="18" t="s">
@@ -8259,13 +8313,13 @@
       <c r="D75" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E75" s="40" t="s">
+      <c r="E75" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="F75" s="40" t="s">
+      <c r="F75" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="G75" s="40" t="s">
+      <c r="G75" s="38" t="s">
         <v>109</v>
       </c>
       <c r="H75" s="19" t="s">
@@ -8280,14 +8334,14 @@
       <c r="K75" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="L75" s="45"/>
+      <c r="L75" s="43"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B76" s="27" t="s">
-        <v>278</v>
+      <c r="B76" s="46" t="s">
+        <v>276</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>34</v>
@@ -8302,28 +8356,28 @@
         <v>275</v>
       </c>
       <c r="G76" s="28">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>276</v>
+        <v>346</v>
       </c>
       <c r="I76" s="29" t="s">
-        <v>277</v>
-      </c>
-      <c r="J76" s="25" t="s">
-        <v>276</v>
+        <v>347</v>
+      </c>
+      <c r="J76" s="29" t="s">
+        <v>346</v>
       </c>
       <c r="K76" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L76" s="45"/>
+      <c r="L76" s="43"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C77" s="24" t="s">
         <v>34</v>
@@ -8335,31 +8389,31 @@
         <v>100</v>
       </c>
       <c r="F77" s="28" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G77" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H77" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I77" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="I77" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="J77" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K77" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L77" s="45"/>
+      <c r="L77" s="43"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C78" s="24" t="s">
         <v>34</v>
@@ -8371,26 +8425,26 @@
         <v>100</v>
       </c>
       <c r="F78" s="28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G78" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H78" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I78" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="I78" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="J78" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K78" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L78" s="45"/>
+      <c r="L78" s="43"/>
       <c r="M78" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -8398,7 +8452,7 @@
         <v>3</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C79" s="24" t="s">
         <v>34</v>
@@ -8410,32 +8464,32 @@
         <v>100</v>
       </c>
       <c r="F79" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G79" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H79" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I79" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="I79" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="J79" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K79" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L79" s="45"/>
+      <c r="L79" s="43"/>
       <c r="M79" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="26"/>
       <c r="B80" s="27" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C80" s="24" t="s">
         <v>34</v>
@@ -8447,32 +8501,32 @@
         <v>100</v>
       </c>
       <c r="F80" s="28" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G80" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H80" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I80" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="I80" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="J80" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K80" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L80" s="45"/>
-      <c r="M80" s="41"/>
+      <c r="L80" s="43"/>
+      <c r="M80" s="39"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C81" s="24" t="s">
         <v>34</v>
@@ -8484,29 +8538,29 @@
         <v>100</v>
       </c>
       <c r="F81" s="28" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G81" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H81" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I81" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="I81" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="J81" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K81" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L81" s="45"/>
+      <c r="L81" s="43"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="26"/>
       <c r="B82" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C82" s="24" t="s">
         <v>34</v>
@@ -8518,31 +8572,31 @@
         <v>100</v>
       </c>
       <c r="F82" s="28" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G82" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H82" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I82" s="29" t="s">
         <v>288</v>
       </c>
-      <c r="I82" s="29" t="s">
-        <v>290</v>
-      </c>
       <c r="J82" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K82" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L82" s="45"/>
+      <c r="L82" s="43"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C83" s="24" t="s">
         <v>34</v>
@@ -8554,26 +8608,26 @@
         <v>100</v>
       </c>
       <c r="F83" s="28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G83" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H83" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="I83" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="I83" s="29" t="s">
-        <v>291</v>
-      </c>
       <c r="J83" s="29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K83" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L83" s="45"/>
+      <c r="L83" s="43"/>
       <c r="M83" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -8581,7 +8635,7 @@
         <v>3</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C84" s="24" t="s">
         <v>34</v>
@@ -8593,31 +8647,31 @@
         <v>100</v>
       </c>
       <c r="F84" s="28" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G84" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H84" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="I84" s="29" t="s">
         <v>289</v>
       </c>
-      <c r="I84" s="29" t="s">
-        <v>291</v>
-      </c>
       <c r="J84" s="29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K84" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L84" s="45"/>
+      <c r="L84" s="43"/>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C85" s="24" t="s">
         <v>34</v>
@@ -8629,31 +8683,31 @@
         <v>100</v>
       </c>
       <c r="F85" s="28" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G85" s="28" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="I85" s="29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J85" s="25" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K85" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L85" s="45"/>
+      <c r="L85" s="43"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C86" s="24" t="s">
         <v>34</v>
@@ -8662,34 +8716,34 @@
         <v>79</v>
       </c>
       <c r="E86" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="G86" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="F86" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="G86" s="16" t="s">
-        <v>301</v>
-      </c>
       <c r="H86" s="29" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="I86" s="29" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="K86" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="L86" s="45"/>
+        <v>348</v>
+      </c>
+      <c r="L86" s="43"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C87" s="24" t="s">
         <v>34</v>
@@ -8701,24 +8755,24 @@
         <v>100</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G87" s="28"/>
       <c r="H87" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I87" s="29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K87" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L87" s="45"/>
+      <c r="L87" s="43"/>
       <c r="M87" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
@@ -8726,7 +8780,7 @@
         <v>3</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C88" s="24" t="s">
         <v>34</v>
@@ -8738,24 +8792,24 @@
         <v>100</v>
       </c>
       <c r="F88" s="28" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G88" s="28"/>
       <c r="H88" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I88" s="29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="K88" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L88" s="45"/>
+      <c r="L88" s="43"/>
       <c r="M88" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
@@ -8763,7 +8817,7 @@
         <v>3</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C89" s="24" t="s">
         <v>34</v>
@@ -8774,25 +8828,25 @@
       <c r="E89" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="F89" s="28" t="s">
-        <v>328</v>
+      <c r="F89" s="16" t="s">
+        <v>326</v>
       </c>
       <c r="G89" s="28"/>
       <c r="H89" s="29" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I89" s="29" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K89" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L89" s="46"/>
+      <c r="L89" s="44"/>
       <c r="M89" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
@@ -8800,7 +8854,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C90" s="24" t="s">
         <v>34</v>
@@ -8812,26 +8866,26 @@
         <v>100</v>
       </c>
       <c r="F90" s="28" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G90" s="28" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="H90" s="29" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I90" s="29" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J90" s="25" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K90" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L90" s="46"/>
+      <c r="L90" s="44"/>
       <c r="M90" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
@@ -8839,7 +8893,7 @@
         <v>3</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C91" s="24" t="s">
         <v>34</v>
@@ -8851,26 +8905,26 @@
         <v>45</v>
       </c>
       <c r="F91" s="28" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G91" s="28">
         <v>95</v>
       </c>
       <c r="H91" s="29" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="I91" s="29" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>324</v>
+        <v>353</v>
       </c>
       <c r="K91" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L91" s="46"/>
+      <c r="L91" s="44"/>
       <c r="M91" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.25">
@@ -8878,7 +8932,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C92" s="24" t="s">
         <v>34</v>
@@ -8890,29 +8944,29 @@
         <v>100</v>
       </c>
       <c r="F92" s="28" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G92" s="28"/>
       <c r="H92" s="29" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="I92" s="29" t="s">
-        <v>335</v>
+        <v>351</v>
       </c>
       <c r="J92" s="29" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
       <c r="K92" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L92" s="46"/>
+      <c r="L92" s="44"/>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C93" s="24" t="s">
         <v>34</v>
@@ -8924,32 +8978,32 @@
         <v>100</v>
       </c>
       <c r="F93" s="28" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G93" s="28"/>
       <c r="H93" s="29" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="I93" s="29" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="J93" s="25" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="K93" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L93" s="46"/>
-      <c r="M93" s="42" t="s">
-        <v>339</v>
+      <c r="L93" s="44"/>
+      <c r="M93" s="40" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B94" s="27" t="s">
-        <v>348</v>
+      <c r="B94" s="46" t="s">
+        <v>342</v>
       </c>
       <c r="C94" s="24" t="s">
         <v>34</v>
@@ -8961,27 +9015,67 @@
         <v>100</v>
       </c>
       <c r="F94" s="28" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G94" s="28" t="s">
         <v>132</v>
       </c>
       <c r="H94" s="29" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="I94" s="25" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="J94" s="29" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="K94" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="L94" s="45"/>
+      <c r="L94" s="43"/>
       <c r="M94" t="s">
-        <v>351</v>
-      </c>
+        <v>345</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E95" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F95" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="G95" s="16"/>
+      <c r="H95" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="I95" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="J95" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="K95" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L95" s="44"/>
+      <c r="M95" s="40" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added variations of the mods Huge, mini, fury_size
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Mods.xlsx
+++ b/Docs/Content/HungryDragonContent_Mods.xlsx
@@ -3413,7 +3413,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="365">
   <si>
     <t>[sku]</t>
   </si>
@@ -4487,6 +4487,27 @@
   </si>
   <si>
     <t>area1:SP_Medieval_Final_Village_Forest_Jalapeno_Invasion;area2:SP_Medieval_Final_Castle_Market_Jalapeno_Invasion;area3:SP_Medieval_Final_Dark_Jalapeno_Invasion</t>
+  </si>
+  <si>
+    <t>fury_size_mod_300</t>
+  </si>
+  <si>
+    <t>huge_1,8</t>
+  </si>
+  <si>
+    <t>mini_0,8</t>
+  </si>
+  <si>
+    <t>mini_0,6</t>
+  </si>
+  <si>
+    <t>fury_size_mod_600</t>
+  </si>
+  <si>
+    <t>huge_1,5</t>
+  </si>
+  <si>
+    <t>fury_size_mod_50</t>
   </si>
 </sst>
 </file>
@@ -4798,7 +4819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4932,6 +4953,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5456,8 +5486,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K95" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
-  <autoFilter ref="A3:K95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A3:K102" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+  <autoFilter ref="A3:K102"/>
   <sortState ref="A4:J34">
     <sortCondition ref="B3:B34"/>
   </sortState>
@@ -5744,10 +5774,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95:J95"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9075,7 +9105,242 @@
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L96"/>
+      <c r="A96" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B96" s="30" t="s">
+        <v>361</v>
+      </c>
+      <c r="C96" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D96" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E96" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F96" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="G96" s="32"/>
+      <c r="H96" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="I96" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="J96" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="K96" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="L96" s="43"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" s="30" t="s">
+        <v>360</v>
+      </c>
+      <c r="C97" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F97" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="G97" s="32"/>
+      <c r="H97" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="I97" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="J97" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="K97" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="L97" s="43"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" s="30" t="s">
+        <v>359</v>
+      </c>
+      <c r="C98" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E98" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F98" s="32">
+        <v>1.8</v>
+      </c>
+      <c r="G98" s="32"/>
+      <c r="H98" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="I98" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="J98" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="K98" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="L98" s="43"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>363</v>
+      </c>
+      <c r="C99" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D99" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E99" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F99" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="G99" s="32"/>
+      <c r="H99" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="I99" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="J99" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="K99" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="L99" s="43"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="C100" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D100" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E100" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="F100" s="28">
+        <v>300</v>
+      </c>
+      <c r="G100" s="28"/>
+      <c r="H100" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="I100" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="J100" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="K100" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L100" s="43"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B101" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="C101" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D101" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E101" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="F101" s="28">
+        <v>600</v>
+      </c>
+      <c r="G101" s="28"/>
+      <c r="H101" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="I101" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="J101" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="K101" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L101" s="43"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E102" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="F102" s="28">
+        <v>50</v>
+      </c>
+      <c r="G102" s="28"/>
+      <c r="H102" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="I102" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="J102" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="K102" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="L102" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>